<commit_message>
Update to OP and RPJ
</commit_message>
<xml_diff>
--- a/OP.xlsx
+++ b/OP.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="81">
   <si>
     <t xml:space="preserve">L/H</t>
   </si>
@@ -136,121 +136,133 @@
     <t xml:space="preserve">MYA</t>
   </si>
   <si>
+    <t xml:space="preserve">ANV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XOV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDYV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDAV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ADD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDRI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLR</t>
+  </si>
+  <si>
     <t xml:space="preserve">ANI</t>
   </si>
   <si>
     <t xml:space="preserve">XOI</t>
   </si>
   <si>
-    <t xml:space="preserve">OUX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CALL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDYV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDAV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RET</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ORA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HLT</t>
+    <t xml:space="preserve">OUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STR</t>
   </si>
   <si>
     <t xml:space="preserve">ORI</t>
   </si>
   <si>
     <t xml:space="preserve">NOI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ADD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LDRI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MOV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XOR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CLR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OUT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STR</t>
   </si>
 </sst>
 </file>
@@ -332,7 +344,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -346,10 +358,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -372,11 +380,11 @@
   </sheetPr>
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J5" activeCellId="0" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -774,10 +782,10 @@
       <c r="F12" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="3" t="s">
         <v>69</v>
       </c>
       <c r="I12" s="3" t="s">
@@ -815,10 +823,10 @@
       <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="I13" s="3" t="s">
@@ -854,10 +862,10 @@
       <c r="F14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="3" t="s">
         <v>27</v>
       </c>
       <c r="I14" s="3" t="s">
@@ -893,17 +901,17 @@
       <c r="F15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="3" t="s">
         <v>36</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
@@ -917,7 +925,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>41</v>
@@ -927,17 +935,17 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>45</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>46</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
@@ -954,12 +962,12 @@
         <v>49</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>52</v>
       </c>
       <c r="I17" s="3" t="s">
@@ -1009,10 +1017,10 @@
         <v>62</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added few ctrl steps for few instustions
</commit_message>
<xml_diff>
--- a/OP.xlsx
+++ b/OP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zero\8bit-CPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeros\Desktop\8bit-CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FDC089E-0338-404C-BCA5-B85BE2FFB19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F3DBEF-AD7F-4725-8202-27AE16B166E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="94">
   <si>
     <t>L/H</t>
   </si>
@@ -262,6 +262,51 @@
   </si>
   <si>
     <t>CMV</t>
+  </si>
+  <si>
+    <t>ldx</t>
+  </si>
+  <si>
+    <t>ldy</t>
+  </si>
+  <si>
+    <t>oex, ldo</t>
+  </si>
+  <si>
+    <t>oey, ldo</t>
+  </si>
+  <si>
+    <t>oea, ldo</t>
+  </si>
+  <si>
+    <t>oex, ldf</t>
+  </si>
+  <si>
+    <t>oey, ldf</t>
+  </si>
+  <si>
+    <t>CMA ----</t>
+  </si>
+  <si>
+    <t>roe, ldf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  oex, st, sic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  oey, st, sic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  oea, st, sic</t>
+  </si>
+  <si>
+    <t>------------------</t>
+  </si>
+  <si>
+    <t>opl, st, osl, add+1, oph, st, osh, add+1, roe, pll, pic, roe, plh, pic</t>
+  </si>
+  <si>
+    <t>oes, pll, osl, sub-1, aoe, osl, oes, plh, osh, sub-1, aoe, osh</t>
   </si>
 </sst>
 </file>
@@ -303,23 +348,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -335,7 +386,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -631,602 +682,792 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="13" max="13" width="61.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="1">
         <v>0</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="1">
         <v>1</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="1">
         <v>2</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="1">
         <v>3</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="1">
         <v>4</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G1" s="1">
         <v>5</v>
       </c>
-      <c r="H1" s="2">
+      <c r="H1" s="1">
         <v>6</v>
       </c>
-      <c r="I1" s="2">
+      <c r="I1" s="1">
         <v>7</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1" s="1">
         <v>8</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="L2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="L3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="L4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="L5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="L6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="L7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="L8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="L9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>0</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>1</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>3</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>4</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>5</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>6</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>7</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>8</v>
       </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="K11" s="1"/>
+      <c r="L11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O11" s="2"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
         <v>0</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="3" t="s">
         <v>62</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="L12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O12" s="2"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1" t="s">
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="L13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O13" s="2"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1" t="s">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="L14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="1" t="s">
+      <c r="E15" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1" t="s">
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="L15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
         <v>4</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1" t="s">
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1" t="s">
+      <c r="H16" s="3"/>
+      <c r="I16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="L16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>5</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D17" s="4"/>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1" t="s">
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="L17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
         <v>6</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1" t="s">
+      <c r="I18" s="3"/>
+      <c r="J18" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="L18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
         <v>7</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1" t="s">
+      <c r="I19" s="3"/>
+      <c r="J19" s="3" t="s">
         <v>75</v>
       </c>
+      <c r="L19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M21" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L29" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L30" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L31" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="L32" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B35" s="2"/>
+      <c r="B35" s="1"/>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B36" s="2"/>
+      <c r="B36" s="1"/>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
Added model of CPU
</commit_message>
<xml_diff>
--- a/OP.xlsx
+++ b/OP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zeros\Desktop\8bit-CPU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zero\8bit-CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F3DBEF-AD7F-4725-8202-27AE16B166E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E7A954-B637-43CD-9402-C6257DC9C8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="120">
   <si>
     <t>L/H</t>
   </si>
@@ -307,6 +307,84 @@
   </si>
   <si>
     <t>oes, pll, osl, sub-1, aoe, osl, oes, plh, osh, sub-1, aoe, osh</t>
+  </si>
+  <si>
+    <t>oex, ost, oeo, lda</t>
+  </si>
+  <si>
+    <t>oey, ost, oeo, lda</t>
+  </si>
+  <si>
+    <t>oea, ost, oeo, lda</t>
+  </si>
+  <si>
+    <t>roe, stl, inc, roe, sth, inc, oer, oeo, lda</t>
+  </si>
+  <si>
+    <t>PC+ROM</t>
+  </si>
+  <si>
+    <t>INC</t>
+  </si>
+  <si>
+    <t>OER</t>
+  </si>
+  <si>
+    <t>OEL</t>
+  </si>
+  <si>
+    <t>OEH</t>
+  </si>
+  <si>
+    <t>LDL</t>
+  </si>
+  <si>
+    <t>LDH</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>OEX</t>
+  </si>
+  <si>
+    <t>OEY</t>
+  </si>
+  <si>
+    <t>ALU</t>
+  </si>
+  <si>
+    <t>LDAO</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>LDF</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>OE</t>
+  </si>
+  <si>
+    <t>CTRL</t>
+  </si>
+  <si>
+    <t>BUS</t>
+  </si>
+  <si>
+    <t>STACK FOR JMP ADDRESSES</t>
   </si>
 </sst>
 </file>
@@ -336,7 +414,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -344,22 +422,96 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
@@ -368,9 +520,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -386,7 +591,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -682,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33:K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -728,7 +933,7 @@
       <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -1108,28 +1313,28 @@
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="5" t="s">
         <v>68</v>
       </c>
       <c r="L12" s="1" t="s">
@@ -1147,23 +1352,23 @@
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="3" t="s">
+      <c r="D13" s="6"/>
+      <c r="E13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3" t="s">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="1" t="s">
@@ -1181,21 +1386,21 @@
       <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="3" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3" t="s">
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5" t="s">
         <v>30</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -1213,23 +1418,23 @@
       <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="3" t="s">
+      <c r="D15" s="6"/>
+      <c r="E15" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3" t="s">
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5" t="s">
         <v>70</v>
       </c>
       <c r="L15" s="1" t="s">
@@ -1247,23 +1452,23 @@
       <c r="A16" s="1">
         <v>4</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3" t="s">
+      <c r="D16" s="6"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="H16" s="5"/>
+      <c r="I16" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="5" t="s">
         <v>73</v>
       </c>
       <c r="L16" s="1" t="s">
@@ -1281,19 +1486,19 @@
       <c r="A17" s="1">
         <v>5</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="G17" s="3" t="s">
+      <c r="D17" s="6"/>
+      <c r="G17" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3" t="s">
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5" t="s">
         <v>52</v>
       </c>
       <c r="L17" s="1" t="s">
@@ -1311,17 +1516,17 @@
       <c r="A18" s="1">
         <v>6</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="5" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3" t="s">
+      <c r="I18" s="5"/>
+      <c r="J18" s="5" t="s">
         <v>57</v>
       </c>
       <c r="L18" s="1" t="s">
@@ -1338,14 +1543,14 @@
       <c r="A19" s="1">
         <v>7</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="5" t="s">
         <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3" t="s">
+      <c r="I19" s="5"/>
+      <c r="J19" s="5" t="s">
         <v>75</v>
       </c>
       <c r="L19" s="1" t="s">
@@ -1369,11 +1574,11 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L21" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M21" s="6" t="s">
+      <c r="M21" s="4" t="s">
         <v>93</v>
       </c>
       <c r="N21" s="1" t="s">
@@ -1381,10 +1586,19 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D22" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="23"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="H22" s="18"/>
       <c r="L22" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="M22" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N22" s="1" t="s">
@@ -1392,38 +1606,82 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D23" s="24"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="16"/>
       <c r="L23" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="M23" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="N23" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="25"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="16"/>
       <c r="L24" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="M24" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="N24" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G25" s="24"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="J25" s="13"/>
       <c r="L25" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="M25" s="2" t="s">
+        <v>96</v>
+      </c>
       <c r="N25" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G26" s="24"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>100</v>
+      </c>
       <c r="L26" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="M26" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="N26" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="24"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="L27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1431,7 +1689,19 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F28" s="13"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>104</v>
+      </c>
       <c r="L28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1440,37 +1710,219 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="E29" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G29" s="24"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
       <c r="L29" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="G30" s="24"/>
+      <c r="H30" s="16"/>
       <c r="L30" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G31" s="24"/>
+      <c r="H31" s="16"/>
       <c r="L31" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G32" s="24"/>
+      <c r="H32" s="16"/>
       <c r="L32" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G33" s="24"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="J33" s="27"/>
+      <c r="K33" s="13"/>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D34" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="J34" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="K34" s="16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
-    </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D35" s="24"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="J35" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="K35" s="16"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="D36" s="24"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K36" s="16"/>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="J37" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="K37" s="16"/>
+    </row>
+    <row r="38" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="24"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="J38" s="17"/>
+      <c r="K38" s="20"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D39" s="24"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="16"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D40" s="24"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="16"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D41" s="24"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="16"/>
+    </row>
+    <row r="42" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="25"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="24"/>
+      <c r="H42" s="16"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G43" s="24"/>
+      <c r="H43" s="16"/>
+      <c r="I43" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G44" s="24"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G45" s="24"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="J45" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G46" s="24"/>
+      <c r="H46" s="16"/>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G47" s="24"/>
+      <c r="H47" s="16"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G48" s="24"/>
+      <c r="H48" s="16"/>
+    </row>
+    <row r="49" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G49" s="24"/>
+      <c r="H49" s="16"/>
+    </row>
+    <row r="50" spans="7:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G50" s="25"/>
+      <c r="H50" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="21">
+    <mergeCell ref="D34:F42"/>
+    <mergeCell ref="G22:H50"/>
+    <mergeCell ref="D22:F24"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K34:K37"/>
+    <mergeCell ref="I33:K33"/>
     <mergeCell ref="J12:J15"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="B16:B18"/>

</xml_diff>

<commit_message>
OP pins for few OP.
</commit_message>
<xml_diff>
--- a/OP.xlsx
+++ b/OP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zero\8bit-CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E7A954-B637-43CD-9402-C6257DC9C8E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50994BF7-336D-49E1-B2D7-0F6D7ABCF09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="119">
   <si>
     <t>L/H</t>
   </si>
@@ -288,39 +288,9 @@
     <t>CMA ----</t>
   </si>
   <si>
-    <t>roe, ldf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  oex, st, sic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  oey, st, sic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  oea, st, sic</t>
-  </si>
-  <si>
     <t>------------------</t>
   </si>
   <si>
-    <t>opl, st, osl, add+1, oph, st, osh, add+1, roe, pll, pic, roe, plh, pic</t>
-  </si>
-  <si>
-    <t>oes, pll, osl, sub-1, aoe, osl, oes, plh, osh, sub-1, aoe, osh</t>
-  </si>
-  <si>
-    <t>oex, ost, oeo, lda</t>
-  </si>
-  <si>
-    <t>oey, ost, oeo, lda</t>
-  </si>
-  <si>
-    <t>oea, ost, oeo, lda</t>
-  </si>
-  <si>
-    <t>roe, stl, inc, roe, sth, inc, oer, oeo, lda</t>
-  </si>
-  <si>
     <t>PC+ROM</t>
   </si>
   <si>
@@ -385,6 +355,33 @@
   </si>
   <si>
     <t>STACK FOR JMP ADDRESSES</t>
+  </si>
+  <si>
+    <t>lda</t>
+  </si>
+  <si>
+    <t>LDO</t>
+  </si>
+  <si>
+    <t>inc, oer, ldf</t>
+  </si>
+  <si>
+    <t>O1</t>
+  </si>
+  <si>
+    <t>OFE</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>ofe, ldl, oel, st, off, ldh, oeh, st, inc, oer, ldl, inc, oer, ldh</t>
+  </si>
+  <si>
+    <t>ofe, ldl, oe, ldl, off, ldh, oe,</t>
+  </si>
+  <si>
+    <t>-----------------------</t>
   </si>
 </sst>
 </file>
@@ -414,7 +411,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -502,11 +499,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -519,59 +542,70 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -890,7 +924,7 @@
   <dimension ref="A1:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33:K33"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -934,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>6</v>
@@ -1060,7 +1094,7 @@
         <v>31</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>7</v>
@@ -1256,7 +1290,7 @@
         <v>78</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>36</v>
@@ -1299,7 +1333,7 @@
         <v>40</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>44</v>
@@ -1313,36 +1347,34 @@
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="26" t="s">
         <v>68</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="M12" s="2" t="s">
-        <v>88</v>
-      </c>
+      <c r="M12" s="2"/>
       <c r="N12" s="1" t="s">
         <v>50</v>
       </c>
@@ -1352,31 +1384,29 @@
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5" t="s">
+      <c r="D13" s="27"/>
+      <c r="E13" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5" t="s">
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M13" s="2" t="s">
-        <v>89</v>
-      </c>
+      <c r="M13" s="2"/>
       <c r="N13" s="1" t="s">
         <v>9</v>
       </c>
@@ -1386,29 +1416,27 @@
       <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5" t="s">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="5" t="s">
+      <c r="D14" s="27"/>
+      <c r="E14" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5" t="s">
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26" t="s">
         <v>30</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M14" s="2" t="s">
-        <v>90</v>
-      </c>
+      <c r="M14" s="2"/>
       <c r="N14" s="1" t="s">
         <v>19</v>
       </c>
@@ -1418,30 +1446,30 @@
       <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5" t="s">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="5" t="s">
+      <c r="D15" s="27"/>
+      <c r="E15" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5" t="s">
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26" t="s">
         <v>70</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M15" s="2" t="s">
-        <v>92</v>
+      <c r="M15" s="32" t="s">
+        <v>116</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>29</v>
@@ -1452,31 +1480,29 @@
       <c r="A16" s="1">
         <v>4</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="26" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5" t="s">
+      <c r="D16" s="27"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5" t="s">
+      <c r="H16" s="26"/>
+      <c r="I16" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="5" t="s">
+      <c r="J16" s="26" t="s">
         <v>73</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M16" s="2" t="s">
-        <v>92</v>
-      </c>
+      <c r="M16" s="32"/>
       <c r="N16" s="1" t="s">
         <v>37</v>
       </c>
@@ -1486,27 +1512,25 @@
       <c r="A17" s="1">
         <v>5</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="G17" s="5" t="s">
+      <c r="D17" s="27"/>
+      <c r="G17" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5" t="s">
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="26" t="s">
         <v>52</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="2" t="s">
-        <v>92</v>
-      </c>
+      <c r="M17" s="32"/>
       <c r="N17" s="1" t="s">
         <v>45</v>
       </c>
@@ -1516,25 +1540,23 @@
       <c r="A18" s="1">
         <v>6</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="26" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5" t="s">
+      <c r="I18" s="26"/>
+      <c r="J18" s="26" t="s">
         <v>57</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M18" s="2" t="s">
-        <v>92</v>
-      </c>
+      <c r="M18" s="32"/>
       <c r="N18" s="1" t="s">
         <v>51</v>
       </c>
@@ -1543,22 +1565,20 @@
       <c r="A19" s="1">
         <v>7</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="26" t="s">
         <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5" t="s">
+      <c r="I19" s="26"/>
+      <c r="J19" s="26" t="s">
         <v>75</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M19" s="2" t="s">
-        <v>92</v>
-      </c>
+      <c r="M19" s="32"/>
       <c r="N19" s="1" t="s">
         <v>56</v>
       </c>
@@ -1567,9 +1587,7 @@
       <c r="L20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M20" s="2" t="s">
-        <v>92</v>
-      </c>
+      <c r="M20" s="32"/>
       <c r="N20" s="1" t="s">
         <v>60</v>
       </c>
@@ -1579,108 +1597,100 @@
         <v>55</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D22" s="22" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="23"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="H22" s="18"/>
+      <c r="D22" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E22" s="15"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="H22" s="20"/>
       <c r="L22" s="1" t="s">
         <v>59</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D23" s="24"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="21"/>
       <c r="L23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M23" s="2" t="s">
-        <v>94</v>
-      </c>
+      <c r="M23" s="2"/>
       <c r="N23" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="25"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="16"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="21"/>
       <c r="L24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M24" s="2" t="s">
-        <v>95</v>
-      </c>
+      <c r="M24" s="2"/>
       <c r="N24" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G25" s="24"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="J25" s="13"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="J25" s="24"/>
       <c r="L25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M25" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="M25" s="2"/>
       <c r="N25" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G26" s="24"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>100</v>
+      <c r="G26" s="16"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M26" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="M26" s="2"/>
       <c r="N26" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G27" s="24"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>102</v>
+      <c r="G27" s="16"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>42</v>
@@ -1690,17 +1700,17 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E28" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="J28" s="11" t="s">
+      <c r="E28" s="23" t="s">
         <v>104</v>
+      </c>
+      <c r="F28" s="24"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>94</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>5</v>
@@ -1710,217 +1720,225 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="E29" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="G29" s="24"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
+      <c r="E29" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G29" s="16"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
       <c r="L29" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="G30" s="24"/>
-      <c r="H30" s="16"/>
+      <c r="E30" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30" s="16"/>
+      <c r="H30" s="21"/>
       <c r="L30" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G31" s="24"/>
-      <c r="H31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="21"/>
       <c r="L31" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G32" s="24"/>
-      <c r="H32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="21"/>
       <c r="L32" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G33" s="24"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="J33" s="27"/>
-      <c r="K33" s="13"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J33" s="25"/>
+      <c r="K33" s="24"/>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D34" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="14" t="s">
+      <c r="D34" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="15"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="J34" s="14" t="s">
+      <c r="J34" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="K34" s="16" t="s">
-        <v>110</v>
+      <c r="K34" s="21" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="21"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="17"/>
       <c r="F35" s="21"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="14" t="s">
+      <c r="G35" s="16"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="J35" s="14" t="s">
+      <c r="J35" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="K35" s="16"/>
+      <c r="K35" s="21"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="21"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="17"/>
       <c r="F36" s="21"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="14" t="s">
+      <c r="G36" s="16"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="J36" s="14" t="s">
+      <c r="J36" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="K36" s="16"/>
+      <c r="K36" s="21"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="21"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="17"/>
       <c r="F37" s="21"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="14" t="s">
+      <c r="G37" s="16"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="K37" s="21"/>
+    </row>
+    <row r="38" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="16"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J38" s="12"/>
+      <c r="K38" s="13"/>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D39" s="16"/>
+      <c r="E39" s="17"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="21"/>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D40" s="16"/>
+      <c r="E40" s="17"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="21"/>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="D41" s="16"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="16"/>
+      <c r="H41" s="21"/>
+    </row>
+    <row r="42" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="G42" s="16"/>
+      <c r="H42" s="21"/>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G43" s="16"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G44" s="16"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G45" s="16"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="J45" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G46" s="16"/>
+      <c r="H46" s="21"/>
+    </row>
+    <row r="47" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G47" s="16"/>
+      <c r="H47" s="21"/>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G48" s="16"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="7:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G49" s="16"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="J37" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="K37" s="16"/>
-    </row>
-    <row r="38" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="24"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="J38" s="17"/>
-      <c r="K38" s="20"/>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D39" s="24"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="16"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D40" s="24"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="16"/>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D41" s="24"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="16"/>
-    </row>
-    <row r="42" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D42" s="25"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="26"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="16"/>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G43" s="24"/>
-      <c r="H43" s="16"/>
-      <c r="I43" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="J43" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G44" s="24"/>
-      <c r="H44" s="16"/>
-      <c r="I44" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="J44" s="9" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G45" s="24"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="J45" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G46" s="24"/>
-      <c r="H46" s="16"/>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G47" s="24"/>
-      <c r="H47" s="16"/>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G48" s="24"/>
-      <c r="H48" s="16"/>
-    </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.2">
-      <c r="G49" s="24"/>
-      <c r="H49" s="16"/>
-    </row>
-    <row r="50" spans="7:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G50" s="25"/>
-      <c r="H50" s="19"/>
+    </row>
+    <row r="50" spans="7:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G50" s="18"/>
+      <c r="H50" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="D34:F42"/>
-    <mergeCell ref="G22:H50"/>
-    <mergeCell ref="D22:F24"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="I25:J25"/>
+  <mergeCells count="22">
+    <mergeCell ref="M15:M20"/>
     <mergeCell ref="K34:K37"/>
     <mergeCell ref="I33:K33"/>
     <mergeCell ref="J12:J15"/>
@@ -1937,6 +1955,11 @@
     <mergeCell ref="E12:E16"/>
     <mergeCell ref="F12:F16"/>
     <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G22:H50"/>
+    <mergeCell ref="D22:F24"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D34:F41"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
OP pins for every OP
</commit_message>
<xml_diff>
--- a/OP.xlsx
+++ b/OP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zero\8bit-CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50994BF7-336D-49E1-B2D7-0F6D7ABCF09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3474DE-91A0-44D2-8102-CB45F89DDDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="162">
   <si>
     <t>L/H</t>
   </si>
@@ -382,6 +382,135 @@
   </si>
   <si>
     <t>-----------------------</t>
+  </si>
+  <si>
+    <t>inc, oer, ldl, inc, oer, ldh, oex, st</t>
+  </si>
+  <si>
+    <t>inc, oer, ldl, inc, oer, ldh, oea, st</t>
+  </si>
+  <si>
+    <t>inc, oer, ldl, inc, oer, ldh, oey, st</t>
+  </si>
+  <si>
+    <t>OEA</t>
+  </si>
+  <si>
+    <t>OEO</t>
+  </si>
+  <si>
+    <t>oex, ldao, add, oeo, lda</t>
+  </si>
+  <si>
+    <t>oey, ldao, add, oeo, lda</t>
+  </si>
+  <si>
+    <t>oea, ldao, add, oeo, lda</t>
+  </si>
+  <si>
+    <t>inc, oer, ldl, inc, oer, ldh, oe, add, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>inc, oer, add, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>oex, ldao, sub, oeo, lda</t>
+  </si>
+  <si>
+    <t>oey, ldao, sub, oeo, lda</t>
+  </si>
+  <si>
+    <t>oea, ldao, sub, oeo, lda</t>
+  </si>
+  <si>
+    <t>inc, oer, ldl, inc, oer, ldh, oe, sub, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>inc, oer, sub, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>inc, oer, ldx</t>
+  </si>
+  <si>
+    <t>inc, oer, ldy</t>
+  </si>
+  <si>
+    <t>inc, oer, lda</t>
+  </si>
+  <si>
+    <t>inc, oer, ldl, inc, oer, ldh, oe, ldx</t>
+  </si>
+  <si>
+    <t>inc, oer, ldl, inc, oer, ldh, oe, ldy</t>
+  </si>
+  <si>
+    <t>inc, oer, ldl, inc, oer, ldh, oe, lda</t>
+  </si>
+  <si>
+    <t>oex, ldy</t>
+  </si>
+  <si>
+    <t>oex, lda</t>
+  </si>
+  <si>
+    <t>oey, ldx</t>
+  </si>
+  <si>
+    <t>oey, lda</t>
+  </si>
+  <si>
+    <t>oea, ldx</t>
+  </si>
+  <si>
+    <t>oea, ldy</t>
+  </si>
+  <si>
+    <t>oex, and, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>oey, and, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>?????</t>
+  </si>
+  <si>
+    <t>inc, oer, and, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>oex, or, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>oey, or, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>????????</t>
+  </si>
+  <si>
+    <t>inc, oer, or, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>oex, xor, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>oey, xor, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>CLR????????</t>
+  </si>
+  <si>
+    <t>inc, oer, xor, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>oex, not, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>oey, not, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>oea, not, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>inc, oer, not, ldao, oeo, lda</t>
   </si>
 </sst>
 </file>
@@ -529,7 +658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -551,51 +680,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -607,6 +691,56 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,13 +1057,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="13" max="13" width="61.28515625" customWidth="1"/>
+    <col min="15" max="15" width="48.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -973,7 +1108,9 @@
       <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="1"/>
+      <c r="O1" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
@@ -1015,7 +1152,9 @@
       <c r="N2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="2"/>
+      <c r="O2" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -1057,7 +1196,9 @@
       <c r="N3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="O3" s="2"/>
+      <c r="O3" s="1" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -1099,7 +1240,9 @@
       <c r="N4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="2"/>
+      <c r="O4" s="2" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -1141,7 +1284,9 @@
       <c r="N5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="2"/>
+      <c r="O5" s="17" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1183,7 +1328,9 @@
       <c r="N6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="O6" s="2"/>
+      <c r="O6" s="17" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1219,7 +1366,9 @@
       <c r="N7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O7" s="2"/>
+      <c r="O7" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1249,7 +1398,9 @@
       <c r="N8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="2"/>
+      <c r="O8" s="2" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1276,7 +1427,9 @@
       <c r="N9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O9" s="2"/>
+      <c r="O9" s="2" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
@@ -1295,7 +1448,9 @@
       <c r="N10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="O10" s="2"/>
+      <c r="O10" s="2" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -1338,7 +1493,9 @@
       <c r="N11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="O11" s="2"/>
+      <c r="O11" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1347,249 +1504,276 @@
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="26" t="s">
+      <c r="F12" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="26" t="s">
+      <c r="G12" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="26" t="s">
+      <c r="H12" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="26" t="s">
+      <c r="I12" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="23" t="s">
         <v>68</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="M12" s="2"/>
+      <c r="M12" s="2" t="s">
+        <v>119</v>
+      </c>
       <c r="N12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="O12" s="2"/>
+      <c r="O12" s="2" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="26" t="s">
+      <c r="D13" s="24"/>
+      <c r="E13" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="26" t="s">
+      <c r="F13" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26" t="s">
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M13" s="2"/>
+      <c r="M13" s="17" t="s">
+        <v>121</v>
+      </c>
       <c r="N13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O13" s="2"/>
+      <c r="O13" s="2" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26" t="s">
+      <c r="B14" s="23"/>
+      <c r="C14" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="26" t="s">
+      <c r="D14" s="24"/>
+      <c r="E14" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26" t="s">
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23" t="s">
         <v>30</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="M14" s="2"/>
+      <c r="M14" s="17" t="s">
+        <v>120</v>
+      </c>
       <c r="N14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O14" s="2"/>
+      <c r="O14" s="2" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26" t="s">
+      <c r="B15" s="23"/>
+      <c r="C15" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="26" t="s">
+      <c r="D15" s="24"/>
+      <c r="E15" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26" t="s">
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23" t="s">
         <v>70</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M15" s="32" t="s">
+      <c r="M15" s="18" t="s">
         <v>116</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O15" s="2"/>
+      <c r="O15" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>4</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="23" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26" t="s">
+      <c r="D16" s="24"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26" t="s">
+      <c r="H16" s="23"/>
+      <c r="I16" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="23" t="s">
         <v>73</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M16" s="32"/>
+      <c r="M16" s="18"/>
       <c r="N16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="O16" s="2"/>
+      <c r="O16" s="2" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>5</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="G17" s="26" t="s">
+      <c r="D17" s="24"/>
+      <c r="G17" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26" t="s">
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23" t="s">
         <v>52</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="32"/>
+      <c r="M17" s="18"/>
       <c r="N17" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O17" s="2"/>
+      <c r="O17" s="17" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>6</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="23" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26" t="s">
+      <c r="I18" s="23"/>
+      <c r="J18" s="23" t="s">
         <v>57</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M18" s="32"/>
+      <c r="M18" s="18"/>
       <c r="N18" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="O18" s="17" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>7</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="23" t="s">
         <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26" t="s">
+      <c r="I19" s="23"/>
+      <c r="J19" s="23" t="s">
         <v>75</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M19" s="32"/>
+      <c r="M19" s="18"/>
       <c r="N19" s="1" t="s">
         <v>56</v>
+      </c>
+      <c r="O19" s="17" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="L20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M20" s="32"/>
+      <c r="M20" s="18"/>
       <c r="N20" s="1" t="s">
         <v>60</v>
+      </c>
+      <c r="O20" s="17" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -1602,17 +1786,20 @@
       <c r="N21" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="O21" s="17" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="14" t="s">
+      <c r="E22" s="30"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="20"/>
+      <c r="H22" s="26"/>
       <c r="L22" s="1" t="s">
         <v>59</v>
       </c>
@@ -1622,53 +1809,71 @@
       <c r="N22" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="O22" s="17" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D23" s="16"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="21"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="19"/>
       <c r="L23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M23" s="2"/>
+      <c r="M23" s="2" t="s">
+        <v>124</v>
+      </c>
       <c r="N23" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="O23" s="17" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="24" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="18"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="21"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="19"/>
       <c r="L24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M24" s="2"/>
+      <c r="M24" s="17" t="s">
+        <v>125</v>
+      </c>
       <c r="N24" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="O24" s="17" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G25" s="16"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="25" t="s">
+      <c r="G25" s="27"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="J25" s="24"/>
+      <c r="J25" s="22"/>
       <c r="L25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M25" s="2"/>
+      <c r="M25" s="17" t="s">
+        <v>126</v>
+      </c>
       <c r="N25" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="O25" s="17" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G26" s="16"/>
-      <c r="H26" s="21"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="19"/>
       <c r="I26" s="10" t="s">
         <v>89</v>
       </c>
@@ -1678,14 +1883,19 @@
       <c r="L26" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M26" s="2"/>
+      <c r="M26" s="2" t="s">
+        <v>127</v>
+      </c>
       <c r="N26" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="O26" s="17" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="27" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G27" s="16"/>
-      <c r="H27" s="21"/>
+      <c r="G27" s="27"/>
+      <c r="H27" s="19"/>
       <c r="I27" s="10" t="s">
         <v>91</v>
       </c>
@@ -1695,17 +1905,23 @@
       <c r="L27" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="M27" s="17" t="s">
+        <v>128</v>
+      </c>
       <c r="N27" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="O27" s="17" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="28" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="F28" s="24"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="21"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="19"/>
       <c r="I28" s="12" t="s">
         <v>93</v>
       </c>
@@ -1715,8 +1931,14 @@
       <c r="L28" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="M28" s="17" t="s">
+        <v>129</v>
+      </c>
       <c r="N28" s="1" t="s">
         <v>61</v>
+      </c>
+      <c r="O28" s="17" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -1726,13 +1948,16 @@
       <c r="F29" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G29" s="16"/>
-      <c r="H29" s="21"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="19"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="L29" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="M29" s="17" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="30" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E30" s="8" t="s">
@@ -1741,148 +1966,166 @@
       <c r="F30" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="G30" s="16"/>
-      <c r="H30" s="21"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="19"/>
       <c r="L30" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G31" s="16"/>
-      <c r="H31" s="21"/>
+      <c r="M30" s="17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="27"/>
+      <c r="H31" s="19"/>
       <c r="L31" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G32" s="16"/>
-      <c r="H32" s="21"/>
+      <c r="M31" s="17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G32" s="27"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="J32" s="21"/>
+      <c r="K32" s="22"/>
       <c r="L32" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="M32" s="17" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="33" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G33" s="16"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="J33" s="25"/>
-      <c r="K33" s="24"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K33" s="19" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D34" s="14" t="s">
+      <c r="D34" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="10" t="s">
-        <v>63</v>
+      <c r="E34" s="30"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="K34" s="21" t="s">
-        <v>100</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="K34" s="19"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="10" t="s">
-        <v>77</v>
+      <c r="D35" s="27"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="6" t="s">
+        <v>68</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="K35" s="21"/>
+        <v>73</v>
+      </c>
+      <c r="K35" s="19"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="10" t="s">
-        <v>68</v>
+      <c r="D36" s="27"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="K36" s="21"/>
+        <v>102</v>
+      </c>
+      <c r="K36" s="19"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="16"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="J37" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="K37" s="21"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J37" s="10"/>
+      <c r="K37" s="33" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="38" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="16"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="21"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="J38" s="12"/>
-      <c r="K38" s="13"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="K38" s="9"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D39" s="16"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="16"/>
-      <c r="H39" s="21"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="19"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D40" s="16"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="21"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="19"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D41" s="16"/>
-      <c r="E41" s="17"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="21"/>
+      <c r="D41" s="27"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="19"/>
     </row>
     <row r="42" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D42" s="30" t="s">
+      <c r="D42" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="F42" s="31" t="s">
+      <c r="F42" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="G42" s="16"/>
-      <c r="H42" s="21"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="19"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G43" s="16"/>
-      <c r="H43" s="21"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="19"/>
       <c r="I43" s="11" t="s">
         <v>95</v>
       </c>
@@ -1891,8 +2134,8 @@
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G44" s="16"/>
-      <c r="H44" s="21"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="19"/>
       <c r="I44" s="10" t="s">
         <v>97</v>
       </c>
@@ -1901,8 +2144,8 @@
       </c>
     </row>
     <row r="45" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G45" s="16"/>
-      <c r="H45" s="21"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="19"/>
       <c r="I45" s="12" t="s">
         <v>6</v>
       </c>
@@ -1911,36 +2154,42 @@
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G46" s="16"/>
-      <c r="H46" s="21"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="19"/>
     </row>
     <row r="47" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G47" s="16"/>
-      <c r="H47" s="21"/>
+      <c r="G47" s="27"/>
+      <c r="H47" s="19"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G48" s="16"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="28" t="s">
+      <c r="G48" s="27"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="49" spans="7:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G49" s="16"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="29" t="s">
+      <c r="G49" s="27"/>
+      <c r="H49" s="19"/>
+      <c r="I49" s="14" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="50" spans="7:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G50" s="18"/>
-      <c r="H50" s="22"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G22:H50"/>
+    <mergeCell ref="D22:F24"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D34:F41"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="K33:K36"/>
     <mergeCell ref="M15:M20"/>
-    <mergeCell ref="K34:K37"/>
-    <mergeCell ref="I33:K33"/>
     <mergeCell ref="J12:J15"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="B16:B18"/>
@@ -1954,15 +2203,9 @@
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="E12:E16"/>
     <mergeCell ref="F12:F16"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G22:H50"/>
-    <mergeCell ref="D22:F24"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="D34:F41"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Better table for instructio/Tring
</commit_message>
<xml_diff>
--- a/OP.xlsx
+++ b/OP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zero\8bit-CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3474DE-91A0-44D2-8102-CB45F89DDDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41C4CF9-43D2-4C49-A0D7-ABA5A830CD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="218">
   <si>
     <t>L/H</t>
   </si>
@@ -511,13 +511,181 @@
   </si>
   <si>
     <t>inc, oer, not, ldao, oeo, lda</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>T5</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>inc</t>
+  </si>
+  <si>
+    <t>oer, ldf</t>
+  </si>
+  <si>
+    <t>ofe</t>
+  </si>
+  <si>
+    <t>ldl</t>
+  </si>
+  <si>
+    <t>oel, st</t>
+  </si>
+  <si>
+    <t>off, ldh</t>
+  </si>
+  <si>
+    <t>oeh, st</t>
+  </si>
+  <si>
+    <t>oer,ldl</t>
+  </si>
+  <si>
+    <t>oer,ldh</t>
+  </si>
+  <si>
+    <t>oer, ldl</t>
+  </si>
+  <si>
+    <t>oer, ldh</t>
+  </si>
+  <si>
+    <t>oex, st</t>
+  </si>
+  <si>
+    <t>oey, st</t>
+  </si>
+  <si>
+    <t>oea, st</t>
+  </si>
+  <si>
+    <t>oe, ldl</t>
+  </si>
+  <si>
+    <t>oe, ldh</t>
+  </si>
+  <si>
+    <t>ofe, ldl</t>
+  </si>
+  <si>
+    <t>oex,  add, ldao</t>
+  </si>
+  <si>
+    <t>oeao, lda</t>
+  </si>
+  <si>
+    <t>oey,  add, ldao</t>
+  </si>
+  <si>
+    <t>oea,  add, ldao</t>
+  </si>
+  <si>
+    <t>oe, add, ldao</t>
+  </si>
+  <si>
+    <t>oer, add ,ldao</t>
+  </si>
+  <si>
+    <t>oex,  sub, ldao</t>
+  </si>
+  <si>
+    <t>oey,  sub, ldao</t>
+  </si>
+  <si>
+    <t>oea, sub, ldao</t>
+  </si>
+  <si>
+    <t>oe, sub, ldao</t>
+  </si>
+  <si>
+    <t>oer, sub ,ldao</t>
+  </si>
+  <si>
+    <t>inc, oer</t>
+  </si>
+  <si>
+    <t>oe, ldx</t>
+  </si>
+  <si>
+    <t>oe, ldy</t>
+  </si>
+  <si>
+    <t>oe,lda</t>
+  </si>
+  <si>
+    <t>oex, and, ldao</t>
+  </si>
+  <si>
+    <t>oey, and, ldao</t>
+  </si>
+  <si>
+    <t>oer, and, ldoa</t>
+  </si>
+  <si>
+    <t>oer, or, ldoa</t>
+  </si>
+  <si>
+    <t>oex, or, ldoa</t>
+  </si>
+  <si>
+    <t>oey, or, ldoa</t>
+  </si>
+  <si>
+    <t>oex, xor, ldao</t>
+  </si>
+  <si>
+    <t>oey, xor, ldao</t>
+  </si>
+  <si>
+    <t>oea, xor, ldao</t>
+  </si>
+  <si>
+    <t>oer, xor, ldao</t>
+  </si>
+  <si>
+    <t>oex, not, ldao</t>
+  </si>
+  <si>
+    <t>oey, not, ldao</t>
+  </si>
+  <si>
+    <t>oea, not, ldao</t>
+  </si>
+  <si>
+    <t>oer, not, ldao</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -527,6 +695,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -658,7 +832,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -691,25 +865,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -721,6 +885,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -730,17 +900,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1055,19 +1244,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O50"/>
+  <dimension ref="A1:AV50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AF25" sqref="AF25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="13" max="13" width="61.28515625" customWidth="1"/>
     <col min="15" max="15" width="48.28515625" customWidth="1"/>
+    <col min="24" max="28" width="11.5703125" customWidth="1"/>
+    <col min="29" max="29" width="14.140625" customWidth="1"/>
+    <col min="30" max="30" width="15.5703125" customWidth="1"/>
+    <col min="31" max="31" width="14.28515625" customWidth="1"/>
+    <col min="35" max="35" width="13.42578125" customWidth="1"/>
+    <col min="36" max="36" width="13.5703125" customWidth="1"/>
+    <col min="37" max="37" width="12.5703125" customWidth="1"/>
+    <col min="38" max="38" width="13.28515625" customWidth="1"/>
+    <col min="39" max="39" width="14.5703125" customWidth="1"/>
+    <col min="40" max="40" width="13.85546875" customWidth="1"/>
+    <col min="41" max="41" width="14.140625" customWidth="1"/>
+    <col min="42" max="42" width="14.5703125" customWidth="1"/>
+    <col min="43" max="43" width="14.42578125" customWidth="1"/>
+    <col min="44" max="44" width="14" customWidth="1"/>
+    <col min="45" max="45" width="13.85546875" customWidth="1"/>
+    <col min="46" max="46" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1111,8 +1316,105 @@
       <c r="O1" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" s="40"/>
+      <c r="Q1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="S1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="X1" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y1" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z1" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AA1" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB1" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC1" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="AD1" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF1" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG1" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH1" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ1" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK1" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="AN1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AO1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="AP1" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AT1" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="AU1" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="AV1" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1155,8 +1457,105 @@
       <c r="O2" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q2" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="S2" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y2" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z2" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA2" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB2" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="AC2" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD2" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="AE2" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="AF2" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="AG2" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="AH2" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="AI2" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="AJ2" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="AK2" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="AN2" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="AO2" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="AP2" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AQ2" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AR2" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="AS2" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="AT2" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="AU2" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AV2" s="40" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1199,8 +1598,89 @@
       <c r="O3" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA3" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB3" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC3" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="AD3" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="AE3" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="AF3" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="AG3" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="AH3" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="AI3" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="AJ3" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="AK3" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="AL3" s="38"/>
+      <c r="AM3" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AN3" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AO3" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AP3" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="AQ3" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="AR3" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AS3" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AT3" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AU3" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="AV3" s="40" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1243,8 +1723,73 @@
       <c r="O4" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q4" s="37"/>
+      <c r="R4" s="37"/>
+      <c r="S4" s="37"/>
+      <c r="T4" s="37"/>
+      <c r="U4" s="37"/>
+      <c r="V4" s="37"/>
+      <c r="W4" s="37"/>
+      <c r="X4" s="37"/>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AB4" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AC4" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD4" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AE4" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AF4" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AG4" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AH4" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AI4" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ4" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="AK4" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="AL4" s="38"/>
+      <c r="AM4" s="38"/>
+      <c r="AN4" s="38"/>
+      <c r="AO4" s="38"/>
+      <c r="AP4" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AQ4" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AR4" s="39"/>
+      <c r="AS4" s="39"/>
+      <c r="AT4" s="39"/>
+      <c r="AU4" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AV4" s="40" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1287,8 +1832,69 @@
       <c r="O5" s="17" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q5" s="37"/>
+      <c r="R5" s="37"/>
+      <c r="S5" s="37"/>
+      <c r="T5" s="37"/>
+      <c r="U5" s="37"/>
+      <c r="V5" s="37"/>
+      <c r="W5" s="37"/>
+      <c r="X5" s="37"/>
+      <c r="Y5" s="37"/>
+      <c r="Z5" s="38"/>
+      <c r="AA5" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="AB5" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="AC5" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD5" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="AE5" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="AF5" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="AG5" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="AH5" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="AI5" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ5" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="AK5" s="40" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL5" s="38"/>
+      <c r="AM5" s="38"/>
+      <c r="AN5" s="38"/>
+      <c r="AO5" s="38"/>
+      <c r="AP5" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="AQ5" s="38"/>
+      <c r="AR5" s="38"/>
+      <c r="AS5" s="38"/>
+      <c r="AT5" s="38"/>
+      <c r="AU5" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="AV5" s="38"/>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1331,8 +1937,67 @@
       <c r="O6" s="17" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P6" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37"/>
+      <c r="X6" s="37"/>
+      <c r="Y6" s="37"/>
+      <c r="Z6" s="38"/>
+      <c r="AA6" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB6" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="AC6" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="AD6" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="AE6" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="AF6" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="AG6" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="AH6" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="AI6" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="AJ6" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="AK6" s="38"/>
+      <c r="AL6" s="38"/>
+      <c r="AM6" s="38"/>
+      <c r="AN6" s="38"/>
+      <c r="AO6" s="38"/>
+      <c r="AP6" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="AQ6" s="38"/>
+      <c r="AR6" s="38"/>
+      <c r="AS6" s="38"/>
+      <c r="AT6" s="38"/>
+      <c r="AU6" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="AV6" s="38"/>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1369,8 +2034,61 @@
       <c r="O7" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P7" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="37"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="37"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37"/>
+      <c r="X7" s="37"/>
+      <c r="Y7" s="37"/>
+      <c r="Z7" s="38"/>
+      <c r="AA7" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB7" s="38"/>
+      <c r="AC7" s="38"/>
+      <c r="AD7" s="38"/>
+      <c r="AE7" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF7" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG7" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AH7" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AI7" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AJ7" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AK7" s="38"/>
+      <c r="AL7" s="38"/>
+      <c r="AM7" s="38"/>
+      <c r="AN7" s="38"/>
+      <c r="AO7" s="38"/>
+      <c r="AP7" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AQ7" s="38"/>
+      <c r="AR7" s="38"/>
+      <c r="AS7" s="38"/>
+      <c r="AT7" s="38"/>
+      <c r="AU7" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AV7" s="38"/>
+    </row>
+    <row r="8" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1401,8 +2119,57 @@
       <c r="O8" s="2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P8" s="18" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="37"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="37"/>
+      <c r="U8" s="37"/>
+      <c r="V8" s="37"/>
+      <c r="W8" s="37"/>
+      <c r="X8" s="37"/>
+      <c r="Y8" s="37"/>
+      <c r="Z8" s="38"/>
+      <c r="AA8" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="AB8" s="38"/>
+      <c r="AC8" s="38"/>
+      <c r="AD8" s="38"/>
+      <c r="AE8" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="AF8" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="AG8" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="AH8" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="AI8" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="AJ8" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="AK8" s="38"/>
+      <c r="AL8" s="38"/>
+      <c r="AM8" s="38"/>
+      <c r="AN8" s="38"/>
+      <c r="AO8" s="38"/>
+      <c r="AP8" s="38"/>
+      <c r="AQ8" s="38"/>
+      <c r="AR8" s="38"/>
+      <c r="AS8" s="38"/>
+      <c r="AT8" s="38"/>
+      <c r="AU8" s="38"/>
+      <c r="AV8" s="38"/>
+    </row>
+    <row r="9" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1430,8 +2197,57 @@
       <c r="O9" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P9" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37"/>
+      <c r="X9" s="37"/>
+      <c r="Y9" s="37"/>
+      <c r="Z9" s="38"/>
+      <c r="AA9" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AB9" s="38"/>
+      <c r="AC9" s="38"/>
+      <c r="AD9" s="38"/>
+      <c r="AE9" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF9" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AG9" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AH9" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AI9" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AJ9" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AK9" s="38"/>
+      <c r="AL9" s="38"/>
+      <c r="AM9" s="38"/>
+      <c r="AN9" s="38"/>
+      <c r="AO9" s="38"/>
+      <c r="AP9" s="38"/>
+      <c r="AQ9" s="38"/>
+      <c r="AR9" s="38"/>
+      <c r="AS9" s="38"/>
+      <c r="AT9" s="38"/>
+      <c r="AU9" s="38"/>
+      <c r="AV9" s="38"/>
+    </row>
+    <row r="10" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
@@ -1451,8 +2267,57 @@
       <c r="O10" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="37"/>
+      <c r="U10" s="37"/>
+      <c r="V10" s="37"/>
+      <c r="W10" s="37"/>
+      <c r="X10" s="37"/>
+      <c r="Y10" s="37"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="38"/>
+      <c r="AD10" s="38"/>
+      <c r="AE10" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="AF10" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="AG10" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="AH10" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="AI10" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="AJ10" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="AK10" s="38"/>
+      <c r="AL10" s="38"/>
+      <c r="AM10" s="38"/>
+      <c r="AN10" s="38"/>
+      <c r="AO10" s="38"/>
+      <c r="AP10" s="38"/>
+      <c r="AQ10" s="38"/>
+      <c r="AR10" s="38"/>
+      <c r="AS10" s="38"/>
+      <c r="AT10" s="38"/>
+      <c r="AU10" s="38"/>
+      <c r="AV10" s="38"/>
+    </row>
+    <row r="11" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1496,36 +2361,69 @@
       <c r="O11" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P11" s="18"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="37"/>
+      <c r="U11" s="37"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="37"/>
+      <c r="X11" s="37"/>
+      <c r="Y11" s="37"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="38"/>
+      <c r="AB11" s="38"/>
+      <c r="AC11" s="38"/>
+      <c r="AD11" s="38"/>
+      <c r="AE11" s="38"/>
+      <c r="AF11" s="38"/>
+      <c r="AG11" s="38"/>
+      <c r="AH11" s="38"/>
+      <c r="AI11" s="38"/>
+      <c r="AJ11" s="38"/>
+      <c r="AK11" s="38"/>
+      <c r="AL11" s="38"/>
+      <c r="AM11" s="38"/>
+      <c r="AN11" s="38"/>
+      <c r="AO11" s="38"/>
+      <c r="AP11" s="38"/>
+      <c r="AQ11" s="38"/>
+      <c r="AR11" s="38"/>
+      <c r="AS11" s="38"/>
+      <c r="AT11" s="38"/>
+      <c r="AU11" s="38"/>
+      <c r="AV11" s="38"/>
+    </row>
+    <row r="12" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="22" t="s">
         <v>68</v>
       </c>
       <c r="L12" s="1" t="s">
@@ -1540,28 +2438,61 @@
       <c r="O12" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P12" s="18"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="37"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="37"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="37"/>
+      <c r="W12" s="37"/>
+      <c r="X12" s="37"/>
+      <c r="Y12" s="37"/>
+      <c r="Z12" s="38"/>
+      <c r="AA12" s="38"/>
+      <c r="AB12" s="38"/>
+      <c r="AC12" s="38"/>
+      <c r="AD12" s="38"/>
+      <c r="AE12" s="38"/>
+      <c r="AF12" s="38"/>
+      <c r="AG12" s="38"/>
+      <c r="AH12" s="38"/>
+      <c r="AI12" s="38"/>
+      <c r="AJ12" s="38"/>
+      <c r="AK12" s="38"/>
+      <c r="AL12" s="38"/>
+      <c r="AM12" s="38"/>
+      <c r="AN12" s="38"/>
+      <c r="AO12" s="38"/>
+      <c r="AP12" s="38"/>
+      <c r="AQ12" s="38"/>
+      <c r="AR12" s="38"/>
+      <c r="AS12" s="38"/>
+      <c r="AT12" s="38"/>
+      <c r="AU12" s="38"/>
+      <c r="AV12" s="38"/>
+    </row>
+    <row r="13" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="23" t="s">
+      <c r="D13" s="36"/>
+      <c r="E13" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="23" t="s">
+      <c r="F13" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23" t="s">
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="1" t="s">
@@ -1576,26 +2507,59 @@
       <c r="O13" s="2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P13" s="18"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="37"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="37"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="37"/>
+      <c r="W13" s="37"/>
+      <c r="X13" s="37"/>
+      <c r="Y13" s="37"/>
+      <c r="Z13" s="38"/>
+      <c r="AA13" s="38"/>
+      <c r="AB13" s="38"/>
+      <c r="AC13" s="38"/>
+      <c r="AD13" s="38"/>
+      <c r="AE13" s="38"/>
+      <c r="AF13" s="38"/>
+      <c r="AG13" s="38"/>
+      <c r="AH13" s="38"/>
+      <c r="AI13" s="38"/>
+      <c r="AJ13" s="38"/>
+      <c r="AK13" s="38"/>
+      <c r="AL13" s="38"/>
+      <c r="AM13" s="38"/>
+      <c r="AN13" s="38"/>
+      <c r="AO13" s="38"/>
+      <c r="AP13" s="38"/>
+      <c r="AQ13" s="38"/>
+      <c r="AR13" s="38"/>
+      <c r="AS13" s="38"/>
+      <c r="AT13" s="38"/>
+      <c r="AU13" s="38"/>
+      <c r="AV13" s="38"/>
+    </row>
+    <row r="14" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23" t="s">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="23" t="s">
+      <c r="D14" s="36"/>
+      <c r="E14" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23" t="s">
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22" t="s">
         <v>30</v>
       </c>
       <c r="L14" s="1" t="s">
@@ -1610,34 +2574,67 @@
       <c r="O14" s="2" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P14" s="18"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="37"/>
+      <c r="W14" s="37"/>
+      <c r="X14" s="37"/>
+      <c r="Y14" s="37"/>
+      <c r="Z14" s="38"/>
+      <c r="AA14" s="38"/>
+      <c r="AB14" s="38"/>
+      <c r="AC14" s="38"/>
+      <c r="AD14" s="38"/>
+      <c r="AE14" s="38"/>
+      <c r="AF14" s="38"/>
+      <c r="AG14" s="38"/>
+      <c r="AH14" s="38"/>
+      <c r="AI14" s="38"/>
+      <c r="AJ14" s="38"/>
+      <c r="AK14" s="38"/>
+      <c r="AL14" s="38"/>
+      <c r="AM14" s="38"/>
+      <c r="AN14" s="38"/>
+      <c r="AO14" s="38"/>
+      <c r="AP14" s="38"/>
+      <c r="AQ14" s="38"/>
+      <c r="AR14" s="38"/>
+      <c r="AS14" s="38"/>
+      <c r="AT14" s="38"/>
+      <c r="AU14" s="38"/>
+      <c r="AV14" s="38"/>
+    </row>
+    <row r="15" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23" t="s">
+      <c r="B15" s="22"/>
+      <c r="C15" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="23" t="s">
+      <c r="D15" s="36"/>
+      <c r="E15" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23" t="s">
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22" t="s">
         <v>70</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M15" s="18" t="s">
+      <c r="M15" s="35" t="s">
         <v>116</v>
       </c>
       <c r="N15" s="1" t="s">
@@ -1646,137 +2643,505 @@
       <c r="O15" s="2" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P15" s="18"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="37"/>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="37"/>
+      <c r="Z15" s="38"/>
+      <c r="AA15" s="38"/>
+      <c r="AB15" s="38"/>
+      <c r="AC15" s="38"/>
+      <c r="AD15" s="38"/>
+      <c r="AE15" s="38"/>
+      <c r="AF15" s="38"/>
+      <c r="AG15" s="38"/>
+      <c r="AH15" s="38"/>
+      <c r="AI15" s="38"/>
+      <c r="AJ15" s="38"/>
+      <c r="AK15" s="38"/>
+      <c r="AL15" s="38"/>
+      <c r="AM15" s="38"/>
+      <c r="AN15" s="38"/>
+      <c r="AO15" s="38"/>
+      <c r="AP15" s="38"/>
+      <c r="AQ15" s="38"/>
+      <c r="AR15" s="38"/>
+      <c r="AS15" s="38"/>
+      <c r="AT15" s="38"/>
+      <c r="AU15" s="38"/>
+      <c r="AV15" s="38"/>
+    </row>
+    <row r="16" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>4</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="22" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23" t="s">
+      <c r="D16" s="36"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23" t="s">
+      <c r="H16" s="22"/>
+      <c r="I16" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="22" t="s">
         <v>73</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M16" s="18"/>
+      <c r="M16" s="35"/>
       <c r="N16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="O16" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P16" s="40"/>
+      <c r="Q16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X16" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z16" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE16" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AI16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AJ16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AL16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AM16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AN16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AO16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AS16" s="40"/>
+      <c r="AT16" s="40"/>
+      <c r="AU16" s="40"/>
+      <c r="AV16" s="40"/>
+    </row>
+    <row r="17" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>5</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="24"/>
-      <c r="G17" s="23" t="s">
+      <c r="D17" s="36"/>
+      <c r="G17" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23" t="s">
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22" t="s">
         <v>52</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="18"/>
+      <c r="M17" s="35"/>
       <c r="N17" s="1" t="s">
         <v>45</v>
       </c>
       <c r="O17" s="17" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P17" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="Q17" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="R17" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="S17" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="T17" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="U17" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="V17" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="W17" s="40" t="s">
+        <v>142</v>
+      </c>
+      <c r="X17" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y17" s="40" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z17" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA17" s="40" t="s">
+        <v>141</v>
+      </c>
+      <c r="AB17" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC17" s="40" t="s">
+        <v>204</v>
+      </c>
+      <c r="AD17" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="AE17" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF17" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="AG17" s="40" t="s">
+        <v>209</v>
+      </c>
+      <c r="AH17" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AI17" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="AJ17" s="40" t="s">
+        <v>211</v>
+      </c>
+      <c r="AK17" s="40" t="s">
+        <v>212</v>
+      </c>
+      <c r="AL17" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AM17" s="40" t="s">
+        <v>214</v>
+      </c>
+      <c r="AN17" s="40" t="s">
+        <v>215</v>
+      </c>
+      <c r="AO17" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="AP17" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="AQ17" s="40"/>
+      <c r="AR17" s="40"/>
+      <c r="AS17" s="40"/>
+      <c r="AT17" s="40"/>
+      <c r="AU17" s="40"/>
+      <c r="AV17" s="40"/>
+    </row>
+    <row r="18" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>6</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="22" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23" t="s">
+      <c r="I18" s="22"/>
+      <c r="J18" s="22" t="s">
         <v>57</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M18" s="18"/>
+      <c r="M18" s="35"/>
       <c r="N18" s="1" t="s">
         <v>51</v>
       </c>
       <c r="O18" s="17" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P18" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q18" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="R18" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="S18" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="T18" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="U18" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="V18" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="W18" s="40"/>
+      <c r="X18" s="40"/>
+      <c r="Y18" s="40"/>
+      <c r="Z18" s="40"/>
+      <c r="AA18" s="40"/>
+      <c r="AB18" s="40"/>
+      <c r="AC18" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD18" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AE18" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="AF18" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AG18" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AH18" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="AI18" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AJ18" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AK18" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AL18" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="AM18" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AN18" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AO18" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AP18" s="40" t="s">
+        <v>217</v>
+      </c>
+      <c r="AQ18" s="40"/>
+      <c r="AR18" s="40"/>
+      <c r="AS18" s="40"/>
+      <c r="AT18" s="40"/>
+      <c r="AU18" s="40"/>
+      <c r="AV18" s="40"/>
+    </row>
+    <row r="19" spans="1:48" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>7</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="22" t="s">
         <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23" t="s">
+      <c r="I19" s="22"/>
+      <c r="J19" s="22" t="s">
         <v>75</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M19" s="18"/>
+      <c r="M19" s="35"/>
       <c r="N19" s="1" t="s">
         <v>56</v>
       </c>
       <c r="O19" s="17" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P19" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="U19" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="V19" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="W19" s="40"/>
+      <c r="X19" s="40"/>
+      <c r="Y19" s="40"/>
+      <c r="Z19" s="40"/>
+      <c r="AA19" s="40"/>
+      <c r="AB19" s="40"/>
+      <c r="AC19" s="40"/>
+      <c r="AD19" s="40"/>
+      <c r="AE19" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF19" s="40"/>
+      <c r="AG19" s="40"/>
+      <c r="AH19" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AI19" s="40"/>
+      <c r="AJ19" s="40"/>
+      <c r="AK19" s="40"/>
+      <c r="AL19" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AM19" s="40"/>
+      <c r="AN19" s="40"/>
+      <c r="AO19" s="40"/>
+      <c r="AP19" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="AQ19" s="40"/>
+      <c r="AR19" s="40"/>
+      <c r="AS19" s="40"/>
+      <c r="AT19" s="40"/>
+      <c r="AU19" s="40"/>
+      <c r="AV19" s="40"/>
+    </row>
+    <row r="20" spans="1:48" x14ac:dyDescent="0.2">
       <c r="L20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M20" s="18"/>
+      <c r="M20" s="35"/>
       <c r="N20" s="1" t="s">
         <v>60</v>
       </c>
       <c r="O20" s="17" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P20" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="U20" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="V20" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="W20" s="40"/>
+      <c r="X20" s="40"/>
+      <c r="Y20" s="40"/>
+      <c r="Z20" s="40"/>
+      <c r="AA20" s="40"/>
+      <c r="AB20" s="40"/>
+      <c r="AC20" s="40"/>
+      <c r="AD20" s="40"/>
+      <c r="AE20" s="40"/>
+      <c r="AF20" s="40"/>
+      <c r="AG20" s="40"/>
+      <c r="AH20" s="40"/>
+      <c r="AI20" s="40"/>
+      <c r="AJ20" s="40"/>
+      <c r="AK20" s="40"/>
+      <c r="AL20" s="40"/>
+      <c r="AM20" s="40"/>
+      <c r="AN20" s="40"/>
+      <c r="AO20" s="40"/>
+      <c r="AP20" s="40"/>
+      <c r="AQ20" s="40"/>
+      <c r="AR20" s="40"/>
+      <c r="AS20" s="40"/>
+      <c r="AT20" s="40"/>
+      <c r="AU20" s="40"/>
+      <c r="AV20" s="40"/>
+    </row>
+    <row r="21" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="L21" s="1" t="s">
         <v>55</v>
       </c>
@@ -1789,17 +3154,29 @@
       <c r="O21" s="17" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D22" s="25" t="s">
+      <c r="P21" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="T21" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="U21" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="V21" s="40" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="D22" s="23" t="s">
         <v>109</v>
       </c>
       <c r="E22" s="30"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="25" t="s">
+      <c r="F22" s="24"/>
+      <c r="G22" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="26"/>
+      <c r="H22" s="24"/>
       <c r="L22" s="1" t="s">
         <v>59</v>
       </c>
@@ -1812,13 +3189,14 @@
       <c r="O22" s="17" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="D23" s="27"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="19"/>
+      <c r="P22" s="18"/>
+    </row>
+    <row r="23" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="D23" s="25"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="26"/>
       <c r="L23" s="1" t="s">
         <v>4</v>
       </c>
@@ -1831,13 +3209,14 @@
       <c r="O23" s="17" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P23" s="18"/>
+    </row>
+    <row r="24" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D24" s="28"/>
-      <c r="E24" s="32"/>
+      <c r="E24" s="31"/>
       <c r="F24" s="29"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="19"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="26"/>
       <c r="L24" s="1" t="s">
         <v>14</v>
       </c>
@@ -1850,14 +3229,15 @@
       <c r="O24" s="17" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G25" s="27"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="21" t="s">
+      <c r="P24" s="18"/>
+    </row>
+    <row r="25" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="G25" s="25"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="J25" s="22"/>
+      <c r="J25" s="33"/>
       <c r="L25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1870,10 +3250,11 @@
       <c r="O25" s="17" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G26" s="27"/>
-      <c r="H26" s="19"/>
+      <c r="P25" s="18"/>
+    </row>
+    <row r="26" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="G26" s="25"/>
+      <c r="H26" s="26"/>
       <c r="I26" s="10" t="s">
         <v>89</v>
       </c>
@@ -1892,10 +3273,11 @@
       <c r="O26" s="17" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G27" s="27"/>
-      <c r="H27" s="19"/>
+      <c r="P26" s="18"/>
+    </row>
+    <row r="27" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="25"/>
+      <c r="H27" s="26"/>
       <c r="I27" s="10" t="s">
         <v>91</v>
       </c>
@@ -1914,14 +3296,15 @@
       <c r="O27" s="17" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E28" s="20" t="s">
+      <c r="P27" s="18"/>
+    </row>
+    <row r="28" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="19"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="26"/>
       <c r="I28" s="12" t="s">
         <v>93</v>
       </c>
@@ -1940,16 +3323,17 @@
       <c r="O28" s="17" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P28" s="18"/>
+    </row>
+    <row r="29" spans="1:48" x14ac:dyDescent="0.2">
       <c r="E29" s="6" t="s">
         <v>93</v>
       </c>
       <c r="F29" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G29" s="27"/>
-      <c r="H29" s="19"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="26"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="L29" s="1" t="s">
@@ -1958,26 +3342,28 @@
       <c r="M29" s="17" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P29" s="18"/>
+    </row>
+    <row r="30" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E30" s="8" t="s">
         <v>105</v>
       </c>
       <c r="F30" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="G30" s="27"/>
-      <c r="H30" s="19"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="26"/>
       <c r="L30" s="1" t="s">
         <v>25</v>
       </c>
       <c r="M30" s="17" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G31" s="27"/>
-      <c r="H31" s="19"/>
+      <c r="P30" s="18"/>
+    </row>
+    <row r="31" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G31" s="25"/>
+      <c r="H31" s="26"/>
       <c r="L31" s="1" t="s">
         <v>35</v>
       </c>
@@ -1985,14 +3371,14 @@
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="G32" s="27"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="20" t="s">
+    <row r="32" spans="1:48" x14ac:dyDescent="0.2">
+      <c r="G32" s="25"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="J32" s="21"/>
-      <c r="K32" s="22"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="33"/>
       <c r="L32" s="1" t="s">
         <v>43</v>
       </c>
@@ -2001,114 +3387,114 @@
       </c>
     </row>
     <row r="33" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G33" s="27"/>
-      <c r="H33" s="31"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="27"/>
       <c r="I33" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="K33" s="19" t="s">
+      <c r="K33" s="26" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D34" s="25" t="s">
+      <c r="D34" s="23" t="s">
         <v>107</v>
       </c>
       <c r="E34" s="30"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="31"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="27"/>
       <c r="I34" s="6" t="s">
         <v>77</v>
       </c>
       <c r="J34" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="K34" s="19"/>
+      <c r="K34" s="26"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="31"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="27"/>
       <c r="I35" s="6" t="s">
         <v>68</v>
       </c>
       <c r="J35" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="K35" s="19"/>
+      <c r="K35" s="26"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
-      <c r="D36" s="27"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="31"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="27"/>
       <c r="I36" s="6" t="s">
         <v>101</v>
       </c>
       <c r="J36" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="K36" s="19"/>
+      <c r="K36" s="26"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="31"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="27"/>
       <c r="I37" s="6" t="s">
         <v>103</v>
       </c>
       <c r="J37" s="10"/>
-      <c r="K37" s="33" t="s">
+      <c r="K37" s="19" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="38" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="27"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="34" t="s">
+      <c r="D38" s="25"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="J38" s="35" t="s">
+      <c r="J38" s="21" t="s">
         <v>122</v>
       </c>
       <c r="K38" s="9"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D39" s="27"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="19"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="26"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D40" s="27"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="19"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="26"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D41" s="27"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="19"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="26"/>
     </row>
     <row r="42" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D42" s="15" t="s">
@@ -2120,12 +3506,12 @@
       <c r="F42" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="G42" s="27"/>
-      <c r="H42" s="19"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="26"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G43" s="27"/>
-      <c r="H43" s="19"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="26"/>
       <c r="I43" s="11" t="s">
         <v>95</v>
       </c>
@@ -2134,8 +3520,8 @@
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G44" s="27"/>
-      <c r="H44" s="19"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="26"/>
       <c r="I44" s="10" t="s">
         <v>97</v>
       </c>
@@ -2144,8 +3530,8 @@
       </c>
     </row>
     <row r="45" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G45" s="27"/>
-      <c r="H45" s="19"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="26"/>
       <c r="I45" s="12" t="s">
         <v>6</v>
       </c>
@@ -2154,23 +3540,23 @@
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G46" s="27"/>
-      <c r="H46" s="19"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="26"/>
     </row>
     <row r="47" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G47" s="27"/>
-      <c r="H47" s="19"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="26"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G48" s="27"/>
-      <c r="H48" s="19"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="26"/>
       <c r="I48" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="49" spans="7:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G49" s="27"/>
-      <c r="H49" s="19"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="26"/>
       <c r="I49" s="14" t="s">
         <v>111</v>
       </c>
@@ -2180,15 +3566,8 @@
       <c r="H50" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G22:H50"/>
-    <mergeCell ref="D22:F24"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="D34:F41"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="K33:K36"/>
+  <mergeCells count="23">
+    <mergeCell ref="AR4:AT4"/>
     <mergeCell ref="M15:M20"/>
     <mergeCell ref="J12:J15"/>
     <mergeCell ref="B13:B15"/>
@@ -2203,7 +3582,16 @@
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="E12:E16"/>
     <mergeCell ref="F12:F16"/>
+    <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G22:H50"/>
+    <mergeCell ref="D22:F24"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D34:F41"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="K33:K36"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
Update to OP and added B-out.
</commit_message>
<xml_diff>
--- a/OP.xlsx
+++ b/OP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zero\8bit-CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C85642-0B44-4536-898F-990F9936434B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554684B3-DA27-41D5-822B-31F85EEA2A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="218">
   <si>
     <t>L/H</t>
   </si>
@@ -330,12 +330,6 @@
     <t>LDAO</t>
   </si>
   <si>
-    <t>SL</t>
-  </si>
-  <si>
-    <t>SR</t>
-  </si>
-  <si>
     <t>LDF</t>
   </si>
   <si>
@@ -627,9 +621,6 @@
     <t>oer, sub ,ldao</t>
   </si>
   <si>
-    <t>inc, oer</t>
-  </si>
-  <si>
     <t>oe, ldx</t>
   </si>
   <si>
@@ -679,6 +670,15 @@
   </si>
   <si>
     <t>oer, not, ldao</t>
+  </si>
+  <si>
+    <t>oer,ldx</t>
+  </si>
+  <si>
+    <t>oer,ldy</t>
+  </si>
+  <si>
+    <t>oer,lda</t>
   </si>
 </sst>
 </file>
@@ -832,7 +832,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -885,15 +885,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -929,6 +920,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1247,7 +1250,7 @@
   <dimension ref="A1:AV50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF25" sqref="AF25"/>
+      <selection activeCell="AQ3" sqref="AQ3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1314,7 +1317,7 @@
         <v>6</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="P1" s="24"/>
       <c r="Q1" s="18" t="s">
@@ -1455,13 +1458,13 @@
         <v>16</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Q2" s="22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="R2" s="18" t="s">
         <v>79</v>
@@ -1470,7 +1473,7 @@
         <v>80</v>
       </c>
       <c r="T2" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="U2" s="18" t="s">
         <v>81</v>
@@ -1488,71 +1491,71 @@
         <v>85</v>
       </c>
       <c r="Z2" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA2" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="AA2" s="18" t="s">
-        <v>174</v>
-      </c>
       <c r="AB2" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="AC2" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD2" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE2" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="AC2" s="18" t="s">
+      <c r="AF2" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="AD2" s="18" t="s">
+      <c r="AG2" s="18" t="s">
         <v>172</v>
       </c>
-      <c r="AE2" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="AF2" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="AG2" s="18" t="s">
-        <v>174</v>
-      </c>
       <c r="AH2" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AI2" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AJ2" s="18" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="AK2" s="18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="AL2" s="23"/>
       <c r="AM2" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="AN2" s="24" t="s">
         <v>189</v>
       </c>
-      <c r="AN2" s="24" t="s">
-        <v>191</v>
-      </c>
       <c r="AO2" s="24" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="AP2" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AQ2" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AR2" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="AS2" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="AT2" s="24" t="s">
         <v>195</v>
       </c>
-      <c r="AS2" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="AT2" s="24" t="s">
-        <v>197</v>
-      </c>
       <c r="AU2" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AV2" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:48" x14ac:dyDescent="0.2">
@@ -1596,14 +1599,14 @@
         <v>26</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P3" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Q3" s="22"/>
       <c r="R3" s="22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="S3" s="22"/>
       <c r="T3" s="22"/>
@@ -1613,71 +1616,71 @@
       <c r="X3" s="22"/>
       <c r="Y3" s="22"/>
       <c r="Z3" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="AA3" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="AA3" s="24" t="s">
-        <v>175</v>
-      </c>
       <c r="AB3" s="24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AC3" s="24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AD3" s="24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AE3" s="24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AF3" s="24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AG3" s="24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AH3" s="24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AI3" s="24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AJ3" s="24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AK3" s="24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="AL3" s="23"/>
       <c r="AM3" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AN3" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AO3" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AP3" s="24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AQ3" s="24" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="AR3" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AS3" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AT3" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AU3" s="24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="AV3" s="24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:48" x14ac:dyDescent="0.2">
@@ -1715,16 +1718,16 @@
         <v>31</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="P4" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q4" s="22"/>
       <c r="R4" s="22"/>
@@ -1737,56 +1740,56 @@
       <c r="Y4" s="22"/>
       <c r="Z4" s="23"/>
       <c r="AA4" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AB4" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AC4" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AD4" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AE4" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AF4" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AG4" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AH4" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AI4" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AJ4" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="AK4" s="24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AL4" s="23"/>
       <c r="AM4" s="23"/>
       <c r="AN4" s="23"/>
       <c r="AO4" s="23"/>
       <c r="AP4" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AQ4" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="AR4" s="25"/>
-      <c r="AS4" s="25"/>
-      <c r="AT4" s="25"/>
+        <v>188</v>
+      </c>
+      <c r="AR4" s="38"/>
+      <c r="AS4" s="38"/>
+      <c r="AT4" s="38"/>
       <c r="AU4" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AV4" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:48" x14ac:dyDescent="0.2">
@@ -1830,10 +1833,10 @@
         <v>17</v>
       </c>
       <c r="O5" s="17" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="P5" s="18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
@@ -1846,51 +1849,51 @@
       <c r="Y5" s="22"/>
       <c r="Z5" s="23"/>
       <c r="AA5" s="24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AB5" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AC5" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AD5" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AE5" s="24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AF5" s="24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AG5" s="24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AH5" s="24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AI5" s="24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AJ5" s="24" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="AK5" s="24" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AL5" s="23"/>
       <c r="AM5" s="23"/>
       <c r="AN5" s="23"/>
       <c r="AO5" s="23"/>
       <c r="AP5" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AQ5" s="23"/>
       <c r="AR5" s="23"/>
       <c r="AS5" s="23"/>
       <c r="AT5" s="23"/>
       <c r="AU5" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="AV5" s="23"/>
     </row>
@@ -1935,10 +1938,10 @@
         <v>27</v>
       </c>
       <c r="O6" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="Q6" s="22"/>
       <c r="R6" s="22"/>
@@ -1951,34 +1954,34 @@
       <c r="Y6" s="22"/>
       <c r="Z6" s="23"/>
       <c r="AA6" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AB6" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="AC6" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD6" s="24" t="s">
         <v>183</v>
       </c>
-      <c r="AC6" s="24" t="s">
-        <v>184</v>
-      </c>
-      <c r="AD6" s="24" t="s">
-        <v>185</v>
-      </c>
       <c r="AE6" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AF6" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AG6" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AH6" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AI6" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AJ6" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="AK6" s="23"/>
       <c r="AL6" s="23"/>
@@ -1986,14 +1989,14 @@
       <c r="AN6" s="23"/>
       <c r="AO6" s="23"/>
       <c r="AP6" s="24" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="AQ6" s="23"/>
       <c r="AR6" s="23"/>
       <c r="AS6" s="23"/>
       <c r="AT6" s="23"/>
       <c r="AU6" s="24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="AV6" s="23"/>
     </row>
@@ -2032,10 +2035,10 @@
         <v>8</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Q7" s="22"/>
       <c r="R7" s="22"/>
@@ -2048,28 +2051,28 @@
       <c r="Y7" s="22"/>
       <c r="Z7" s="23"/>
       <c r="AA7" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AB7" s="23"/>
       <c r="AC7" s="23"/>
       <c r="AD7" s="23"/>
       <c r="AE7" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AF7" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AG7" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AH7" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AI7" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AJ7" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AK7" s="23"/>
       <c r="AL7" s="23"/>
@@ -2077,14 +2080,14 @@
       <c r="AN7" s="23"/>
       <c r="AO7" s="23"/>
       <c r="AP7" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AQ7" s="23"/>
       <c r="AR7" s="23"/>
       <c r="AS7" s="23"/>
       <c r="AT7" s="23"/>
       <c r="AU7" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AV7" s="23"/>
     </row>
@@ -2117,10 +2120,10 @@
         <v>18</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
@@ -2133,28 +2136,28 @@
       <c r="Y8" s="22"/>
       <c r="Z8" s="23"/>
       <c r="AA8" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AB8" s="23"/>
       <c r="AC8" s="23"/>
       <c r="AD8" s="23"/>
       <c r="AE8" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AF8" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AG8" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AH8" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AI8" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AJ8" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="AK8" s="23"/>
       <c r="AL8" s="23"/>
@@ -2195,10 +2198,10 @@
         <v>28</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="Q9" s="22"/>
       <c r="R9" s="22"/>
@@ -2211,28 +2214,28 @@
       <c r="Y9" s="22"/>
       <c r="Z9" s="23"/>
       <c r="AA9" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AB9" s="23"/>
       <c r="AC9" s="23"/>
       <c r="AD9" s="23"/>
       <c r="AE9" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AF9" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AG9" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AH9" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AI9" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AJ9" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AK9" s="23"/>
       <c r="AL9" s="23"/>
@@ -2259,16 +2262,16 @@
         <v>78</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N10" s="1" t="s">
         <v>36</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="Q10" s="22"/>
       <c r="R10" s="22"/>
@@ -2281,28 +2284,28 @@
       <c r="Y10" s="22"/>
       <c r="Z10" s="23"/>
       <c r="AA10" s="24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AB10" s="23"/>
       <c r="AC10" s="23"/>
       <c r="AD10" s="23"/>
       <c r="AE10" s="24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AF10" s="24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AG10" s="24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AH10" s="24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AI10" s="24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AJ10" s="24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="AK10" s="23"/>
       <c r="AL10" s="23"/>
@@ -2353,13 +2356,13 @@
         <v>40</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>44</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P11" s="18"/>
       <c r="Q11" s="22"/>
@@ -2402,41 +2405,41 @@
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="27" t="s">
+      <c r="E12" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="27" t="s">
+      <c r="G12" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="27" t="s">
+      <c r="H12" s="40" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="27" t="s">
+      <c r="I12" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="40" t="s">
         <v>68</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>48</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="N12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="P12" s="18"/>
       <c r="Q12" s="22"/>
@@ -2476,36 +2479,36 @@
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="40" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="27" t="s">
+      <c r="D13" s="41"/>
+      <c r="E13" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="27" t="s">
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="M13" s="17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="P13" s="18"/>
       <c r="Q13" s="22"/>
@@ -2545,34 +2548,34 @@
       <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27" t="s">
+      <c r="B14" s="40"/>
+      <c r="C14" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="27" t="s">
+      <c r="D14" s="41"/>
+      <c r="E14" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27" t="s">
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40" t="s">
         <v>30</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>58</v>
       </c>
       <c r="M14" s="17" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="P14" s="18"/>
       <c r="Q14" s="22"/>
@@ -2612,36 +2615,36 @@
       <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="27" t="s">
+      <c r="D15" s="41"/>
+      <c r="E15" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="27" t="s">
+      <c r="G15" s="40" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27" t="s">
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40" t="s">
         <v>70</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M15" s="26" t="s">
-        <v>116</v>
+      <c r="M15" s="39" t="s">
+        <v>114</v>
       </c>
       <c r="N15" s="1" t="s">
         <v>29</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="P15" s="18"/>
       <c r="Q15" s="22"/>
@@ -2681,34 +2684,34 @@
       <c r="A16" s="1">
         <v>4</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="40" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27" t="s">
+      <c r="D16" s="41"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27" t="s">
+      <c r="H16" s="40"/>
+      <c r="I16" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="40" t="s">
         <v>73</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M16" s="26"/>
+      <c r="M16" s="39"/>
       <c r="N16" s="1" t="s">
         <v>37</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="P16" s="24"/>
       <c r="Q16" s="1" t="s">
@@ -2798,111 +2801,111 @@
       <c r="A17" s="1">
         <v>5</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="40" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="G17" s="27" t="s">
+      <c r="D17" s="41"/>
+      <c r="G17" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27" t="s">
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40" t="s">
         <v>52</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M17" s="26"/>
+      <c r="M17" s="39"/>
       <c r="N17" s="1" t="s">
         <v>45</v>
       </c>
       <c r="O17" s="17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P17" s="18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Q17" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="R17" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="S17" s="24" t="s">
-        <v>200</v>
+        <v>170</v>
+      </c>
+      <c r="R17" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="S17" s="25" t="s">
+        <v>170</v>
       </c>
       <c r="T17" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="U17" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="V17" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="W17" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="X17" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="X17" s="24" t="s">
-        <v>144</v>
-      </c>
       <c r="Y17" s="24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Z17" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="AA17" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB17" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="AB17" s="24" t="s">
-        <v>143</v>
-      </c>
       <c r="AC17" s="24" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AD17" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="AE17" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF17" s="24" t="s">
         <v>205</v>
       </c>
-      <c r="AE17" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="AF17" s="24" t="s">
+      <c r="AG17" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="AH17" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI17" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="AJ17" s="24" t="s">
         <v>208</v>
       </c>
-      <c r="AG17" s="24" t="s">
+      <c r="AK17" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="AH17" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="AI17" s="24" t="s">
-        <v>210</v>
-      </c>
-      <c r="AJ17" s="24" t="s">
+      <c r="AL17" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="AM17" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="AK17" s="24" t="s">
+      <c r="AN17" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="AL17" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="AM17" s="24" t="s">
-        <v>214</v>
-      </c>
-      <c r="AN17" s="24" t="s">
-        <v>215</v>
-      </c>
       <c r="AO17" s="24" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="AP17" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="AQ17" s="24"/>
       <c r="AR17" s="24"/>
@@ -2915,49 +2918,49 @@
       <c r="A18" s="1">
         <v>6</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="40" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27" t="s">
+      <c r="I18" s="40"/>
+      <c r="J18" s="40" t="s">
         <v>57</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M18" s="26"/>
+      <c r="M18" s="39"/>
       <c r="N18" s="1" t="s">
         <v>51</v>
       </c>
       <c r="O18" s="17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="P18" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="Q18" s="24" t="s">
-        <v>79</v>
+        <v>215</v>
       </c>
       <c r="R18" s="24" t="s">
-        <v>80</v>
+        <v>216</v>
       </c>
       <c r="S18" s="24" t="s">
-        <v>110</v>
+        <v>217</v>
       </c>
       <c r="T18" s="24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="U18" s="24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="V18" s="24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="W18" s="24"/>
       <c r="X18" s="24"/>
@@ -2966,46 +2969,46 @@
       <c r="AA18" s="24"/>
       <c r="AB18" s="24"/>
       <c r="AC18" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AD18" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AE18" s="24" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="AF18" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AG18" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AH18" s="24" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="AI18" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AJ18" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AK18" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AL18" s="24" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="AM18" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AN18" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AO18" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AP18" s="24" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="AQ18" s="24"/>
       <c r="AR18" s="24"/>
@@ -3018,40 +3021,40 @@
       <c r="A19" s="1">
         <v>7</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="40" t="s">
         <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27" t="s">
+      <c r="I19" s="40"/>
+      <c r="J19" s="40" t="s">
         <v>75</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M19" s="26"/>
+      <c r="M19" s="39"/>
       <c r="N19" s="1" t="s">
         <v>56</v>
       </c>
       <c r="O19" s="17" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="P19" s="18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q19" s="24"/>
       <c r="R19" s="24"/>
       <c r="S19" s="24"/>
       <c r="T19" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="U19" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="V19" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="W19" s="24"/>
       <c r="X19" s="24"/>
@@ -3062,24 +3065,24 @@
       <c r="AC19" s="24"/>
       <c r="AD19" s="24"/>
       <c r="AE19" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AF19" s="24"/>
       <c r="AG19" s="24"/>
       <c r="AH19" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AI19" s="24"/>
       <c r="AJ19" s="24"/>
       <c r="AK19" s="24"/>
       <c r="AL19" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AM19" s="24"/>
       <c r="AN19" s="24"/>
       <c r="AO19" s="24"/>
       <c r="AP19" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="AQ19" s="24"/>
       <c r="AR19" s="24"/>
@@ -3092,27 +3095,27 @@
       <c r="L20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M20" s="26"/>
+      <c r="M20" s="39"/>
       <c r="N20" s="1" t="s">
         <v>60</v>
       </c>
       <c r="O20" s="17" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="P20" s="18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="Q20" s="24"/>
       <c r="R20" s="24"/>
       <c r="S20" s="24"/>
       <c r="T20" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="U20" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="V20" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="W20" s="24"/>
       <c r="X20" s="24"/>
@@ -3146,115 +3149,115 @@
         <v>55</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="N21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="O21" s="17" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="P21" s="18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="T21" s="24" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="U21" s="24" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="V21" s="24" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="D22" s="29" t="s">
-        <v>109</v>
-      </c>
-      <c r="E22" s="36"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="H22" s="30"/>
+      <c r="D22" s="26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="33"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="H22" s="27"/>
       <c r="L22" s="1" t="s">
         <v>59</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="O22" s="17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="P22" s="18"/>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="D23" s="31"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="32"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="29"/>
       <c r="L23" s="1" t="s">
         <v>4</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="N23" s="1" t="s">
         <v>30</v>
       </c>
       <c r="O23" s="17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="P23" s="18"/>
     </row>
     <row r="24" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="34"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="32"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="29"/>
       <c r="L24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="M24" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N24" s="1" t="s">
         <v>38</v>
       </c>
       <c r="O24" s="17" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="P24" s="18"/>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="G25" s="31"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="40" t="s">
+      <c r="G25" s="28"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="37" t="s">
         <v>88</v>
       </c>
-      <c r="J25" s="39"/>
+      <c r="J25" s="36"/>
       <c r="L25" s="1" t="s">
         <v>24</v>
       </c>
       <c r="M25" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="N25" s="1" t="s">
         <v>46</v>
       </c>
       <c r="O25" s="17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="P25" s="18"/>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="G26" s="31"/>
-      <c r="H26" s="32"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="29"/>
       <c r="I26" s="10" t="s">
         <v>89</v>
       </c>
@@ -3265,19 +3268,19 @@
         <v>34</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="N26" s="1" t="s">
         <v>52</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P26" s="18"/>
     </row>
     <row r="27" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G27" s="31"/>
-      <c r="H27" s="32"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="29"/>
       <c r="I27" s="10" t="s">
         <v>91</v>
       </c>
@@ -3288,23 +3291,23 @@
         <v>42</v>
       </c>
       <c r="M27" s="17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>57</v>
       </c>
       <c r="O27" s="17" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P27" s="18"/>
     </row>
     <row r="28" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E28" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="F28" s="39"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="32"/>
+      <c r="E28" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="36"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="29"/>
       <c r="I28" s="12" t="s">
         <v>93</v>
       </c>
@@ -3315,13 +3318,13 @@
         <v>5</v>
       </c>
       <c r="M28" s="17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>61</v>
       </c>
       <c r="O28" s="17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="P28" s="18"/>
     </row>
@@ -3332,186 +3335,182 @@
       <c r="F29" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="G29" s="31"/>
-      <c r="H29" s="32"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="29"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="L29" s="1" t="s">
         <v>15</v>
       </c>
       <c r="M29" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P29" s="18"/>
     </row>
     <row r="30" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E30" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="G30" s="31"/>
-      <c r="H30" s="32"/>
+        <v>104</v>
+      </c>
+      <c r="G30" s="28"/>
+      <c r="H30" s="29"/>
       <c r="L30" s="1" t="s">
         <v>25</v>
       </c>
       <c r="M30" s="17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P30" s="18"/>
     </row>
     <row r="31" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G31" s="31"/>
-      <c r="H31" s="32"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="29"/>
       <c r="L31" s="1" t="s">
         <v>35</v>
       </c>
       <c r="M31" s="17" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="G32" s="31"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="38" t="s">
+      <c r="G32" s="28"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="J32" s="40"/>
-      <c r="K32" s="39"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="36"/>
       <c r="L32" s="1" t="s">
         <v>43</v>
       </c>
       <c r="M32" s="17" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G33" s="31"/>
-      <c r="H33" s="33"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="30"/>
       <c r="I33" s="6" t="s">
         <v>63</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="K33" s="32" t="s">
+      <c r="K33" s="29" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D34" s="29" t="s">
-        <v>107</v>
-      </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="33"/>
+      <c r="D34" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" s="33"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="30"/>
       <c r="I34" s="6" t="s">
         <v>77</v>
       </c>
       <c r="J34" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="K34" s="32"/>
+      <c r="K34" s="29"/>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="33"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="30"/>
       <c r="I35" s="6" t="s">
         <v>68</v>
       </c>
       <c r="J35" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="K35" s="32"/>
+      <c r="K35" s="29"/>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="33"/>
-      <c r="I36" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="J36" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="K36" s="32"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="28"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="29"/>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="33"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="30"/>
       <c r="I37" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="J37" s="10"/>
       <c r="K37" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="31"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="31"/>
-      <c r="H38" s="33"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="30"/>
       <c r="I38" s="20" t="s">
         <v>26</v>
       </c>
       <c r="J38" s="21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K38" s="9"/>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D39" s="31"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="32"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="29"/>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D40" s="31"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="32"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="29"/>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D41" s="31"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="32"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="30"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="28"/>
+      <c r="H41" s="29"/>
     </row>
     <row r="42" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D42" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E42" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="F42" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="E42" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="F42" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="G42" s="31"/>
-      <c r="H42" s="32"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="29"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G43" s="31"/>
-      <c r="H43" s="32"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="29"/>
       <c r="I43" s="11" t="s">
         <v>95</v>
       </c>
@@ -3520,8 +3519,8 @@
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G44" s="31"/>
-      <c r="H44" s="32"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="29"/>
       <c r="I44" s="10" t="s">
         <v>97</v>
       </c>
@@ -3530,8 +3529,8 @@
       </c>
     </row>
     <row r="45" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G45" s="31"/>
-      <c r="H45" s="32"/>
+      <c r="G45" s="28"/>
+      <c r="H45" s="29"/>
       <c r="I45" s="12" t="s">
         <v>6</v>
       </c>
@@ -3540,40 +3539,33 @@
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G46" s="31"/>
-      <c r="H46" s="32"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="29"/>
     </row>
     <row r="47" spans="2:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G47" s="31"/>
-      <c r="H47" s="32"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="29"/>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="G48" s="31"/>
-      <c r="H48" s="32"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="29"/>
       <c r="I48" s="13" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="49" spans="7:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G49" s="31"/>
-      <c r="H49" s="32"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="29"/>
       <c r="I49" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="7:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G50" s="34"/>
-      <c r="H50" s="35"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="G22:H50"/>
-    <mergeCell ref="D22:F24"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="D34:F41"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="K33:K36"/>
     <mergeCell ref="AR4:AT4"/>
     <mergeCell ref="M15:M20"/>
     <mergeCell ref="J12:J15"/>
@@ -3590,6 +3582,13 @@
     <mergeCell ref="E12:E16"/>
     <mergeCell ref="F12:F16"/>
     <mergeCell ref="G15:G17"/>
+    <mergeCell ref="G22:H50"/>
+    <mergeCell ref="D22:F24"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D34:F41"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="K33:K36"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
Small changes to ALU ops
</commit_message>
<xml_diff>
--- a/OP.xlsx
+++ b/OP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zero\8bit-CPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C70207E5-8C24-4A40-938F-5E726A9DB427}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDF8114-D872-432D-B9CB-35F1E89B017E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1605" yWindow="2625" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="191">
   <si>
     <t>L/H</t>
   </si>
@@ -591,13 +591,13 @@
     <t>HCP</t>
   </si>
   <si>
-    <t>LDAO/OEO</t>
-  </si>
-  <si>
     <t>ACP</t>
   </si>
   <si>
     <t>AOE</t>
+  </si>
+  <si>
+    <t>ld</t>
   </si>
 </sst>
 </file>
@@ -830,6 +830,39 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -866,42 +899,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1218,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AV300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38:J38"/>
+    <sheetView tabSelected="1" topLeftCell="A109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1719,9 +1719,9 @@
       <c r="AQ4" s="17" t="s">
         <v>145</v>
       </c>
-      <c r="AR4" s="38"/>
-      <c r="AS4" s="38"/>
-      <c r="AT4" s="38"/>
+      <c r="AR4" s="39"/>
+      <c r="AS4" s="39"/>
+      <c r="AT4" s="39"/>
       <c r="AU4" s="17" t="s">
         <v>129</v>
       </c>
@@ -2271,28 +2271,28 @@
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="41" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="G12" s="40" t="s">
+      <c r="G12" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="40" t="s">
+      <c r="H12" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="40" t="s">
+      <c r="I12" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="J12" s="40" t="s">
+      <c r="J12" s="41" t="s">
         <v>68</v>
       </c>
       <c r="L12" s="1"/>
@@ -2337,23 +2337,23 @@
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="40" t="s">
+      <c r="D13" s="42"/>
+      <c r="E13" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40" t="s">
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41" t="s">
         <v>20</v>
       </c>
       <c r="L13" s="1"/>
@@ -2398,21 +2398,21 @@
       <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40" t="s">
+      <c r="B14" s="41"/>
+      <c r="C14" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="40" t="s">
+      <c r="D14" s="42"/>
+      <c r="E14" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40" t="s">
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41" t="s">
         <v>30</v>
       </c>
       <c r="L14" s="1"/>
@@ -2457,27 +2457,27 @@
       <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40" t="s">
+      <c r="B15" s="41"/>
+      <c r="C15" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="40" t="s">
+      <c r="D15" s="42"/>
+      <c r="E15" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="40" t="s">
+      <c r="G15" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
-      <c r="J15" s="40" t="s">
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41" t="s">
         <v>70</v>
       </c>
       <c r="L15" s="1"/>
-      <c r="M15" s="39"/>
+      <c r="M15" s="40"/>
       <c r="N15" s="1"/>
       <c r="O15" s="2"/>
       <c r="P15" s="14"/>
@@ -2518,27 +2518,27 @@
       <c r="A16" s="1">
         <v>4</v>
       </c>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="41" t="s">
         <v>71</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40" t="s">
+      <c r="D16" s="42"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40" t="s">
+      <c r="H16" s="41"/>
+      <c r="I16" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="J16" s="40" t="s">
+      <c r="J16" s="41" t="s">
         <v>73</v>
       </c>
       <c r="L16" s="1"/>
-      <c r="M16" s="39"/>
+      <c r="M16" s="40"/>
       <c r="N16" s="1"/>
       <c r="O16" s="2"/>
       <c r="P16" s="17"/>
@@ -2629,23 +2629,23 @@
       <c r="A17" s="1">
         <v>5</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="40" t="s">
+      <c r="C17" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="G17" s="40" t="s">
+      <c r="D17" s="42"/>
+      <c r="G17" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40" t="s">
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41" t="s">
         <v>52</v>
       </c>
       <c r="L17" s="1"/>
-      <c r="M17" s="39"/>
+      <c r="M17" s="40"/>
       <c r="N17" s="1"/>
       <c r="O17" s="13"/>
       <c r="P17" s="14" t="s">
@@ -2740,21 +2740,21 @@
       <c r="A18" s="1">
         <v>6</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="40" t="s">
+      <c r="C18" s="41" t="s">
         <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40" t="s">
+      <c r="I18" s="41"/>
+      <c r="J18" s="41" t="s">
         <v>57</v>
       </c>
       <c r="L18" s="1"/>
-      <c r="M18" s="39"/>
+      <c r="M18" s="40"/>
       <c r="N18" s="1"/>
       <c r="O18" s="13"/>
       <c r="P18" s="14" t="s">
@@ -2837,18 +2837,18 @@
       <c r="A19" s="1">
         <v>7</v>
       </c>
-      <c r="C19" s="40" t="s">
+      <c r="C19" s="41" t="s">
         <v>58</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40" t="s">
+      <c r="I19" s="41"/>
+      <c r="J19" s="41" t="s">
         <v>75</v>
       </c>
       <c r="L19" s="1"/>
-      <c r="M19" s="39"/>
+      <c r="M19" s="40"/>
       <c r="N19" s="1"/>
       <c r="O19" s="13"/>
       <c r="P19" s="14" t="s">
@@ -2903,7 +2903,7 @@
     </row>
     <row r="20" spans="1:48" x14ac:dyDescent="0.2">
       <c r="L20" s="1"/>
-      <c r="M20" s="39"/>
+      <c r="M20" s="40"/>
       <c r="N20" s="1"/>
       <c r="O20" s="13"/>
       <c r="P20" s="14" t="s">
@@ -2967,15 +2967,15 @@
       </c>
     </row>
     <row r="22" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="26" t="s">
+      <c r="E22" s="50"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="H22" s="27"/>
+      <c r="H22" s="44"/>
       <c r="L22" s="1"/>
       <c r="M22" s="3"/>
       <c r="N22" s="1"/>
@@ -2983,11 +2983,11 @@
       <c r="P22" s="14"/>
     </row>
     <row r="23" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="D23" s="28"/>
-      <c r="E23" s="30"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="29"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="46"/>
       <c r="L23" s="1"/>
       <c r="M23" s="2"/>
       <c r="N23" s="1"/>
@@ -2995,11 +2995,11 @@
       <c r="P23" s="14"/>
     </row>
     <row r="24" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="31"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="29"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="46"/>
       <c r="L24" s="1"/>
       <c r="M24" s="13"/>
       <c r="N24" s="1"/>
@@ -3007,12 +3007,12 @@
       <c r="P24" s="14"/>
     </row>
     <row r="25" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="G25" s="28"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="37" t="s">
+      <c r="G25" s="45"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="J25" s="36"/>
+      <c r="J25" s="53"/>
       <c r="L25" s="1"/>
       <c r="M25" s="13"/>
       <c r="N25" s="1"/>
@@ -3020,8 +3020,8 @@
       <c r="P25" s="14"/>
     </row>
     <row r="26" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="G26" s="28"/>
-      <c r="H26" s="29"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="46"/>
       <c r="I26" s="21" t="s">
         <v>87</v>
       </c>
@@ -3035,8 +3035,8 @@
       <c r="P26" s="14"/>
     </row>
     <row r="27" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G27" s="28"/>
-      <c r="H27" s="29"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="46"/>
       <c r="I27" s="21" t="s">
         <v>89</v>
       </c>
@@ -3044,100 +3044,100 @@
         <v>90</v>
       </c>
       <c r="L27" s="1"/>
-      <c r="M27" s="46" t="s">
+      <c r="M27" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="N27" s="47" t="s">
+      <c r="N27" s="31" t="s">
         <v>119</v>
       </c>
       <c r="O27" s="13"/>
-      <c r="P27" s="43" t="s">
+      <c r="P27" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="Q27" s="42" t="s">
+      <c r="Q27" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="R27" s="42" t="s">
+      <c r="R27" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="S27" s="42" t="s">
+      <c r="S27" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="T27" s="42" t="s">
+      <c r="T27" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="U27" s="42" t="s">
+      <c r="U27" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="V27" s="45"/>
-      <c r="W27" s="44" t="s">
+      <c r="V27" s="29"/>
+      <c r="W27" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="X27" s="42" t="s">
+      <c r="X27" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="Y27" s="42" t="s">
+      <c r="Y27" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="Z27" s="42" t="s">
+      <c r="Z27" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="AA27" s="42" t="s">
+      <c r="AA27" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="AB27" s="42" t="s">
+      <c r="AB27" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="AC27" s="42" t="s">
+      <c r="AC27" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="AD27" s="42" t="s">
+      <c r="AD27" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="AE27" s="42" t="s">
+      <c r="AE27" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="AF27" s="42" t="s">
+      <c r="AF27" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="AH27" s="44" t="s">
+      <c r="AH27" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="AI27" s="42" t="s">
+      <c r="AI27" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="AJ27" s="42" t="s">
+      <c r="AJ27" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AK27" s="42" t="s">
+      <c r="AK27" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="AL27" s="42" t="s">
+      <c r="AL27" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="AM27" s="42" t="s">
+      <c r="AM27" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="AN27" s="42" t="s">
+      <c r="AN27" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="AO27" s="42" t="s">
+      <c r="AO27" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="AP27" s="42" t="s">
+      <c r="AP27" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="AQ27" s="42" t="s">
+      <c r="AQ27" s="26" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="28" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E28" s="35" t="s">
+      <c r="E28" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="29"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="46"/>
       <c r="I28" s="23" t="s">
         <v>91</v>
       </c>
@@ -3145,14 +3145,14 @@
         <v>92</v>
       </c>
       <c r="L28" s="1"/>
-      <c r="M28" s="46" t="s">
+      <c r="M28" s="30" t="s">
         <v>186</v>
       </c>
-      <c r="N28" s="47" t="s">
+      <c r="N28" s="31" t="s">
         <v>39</v>
       </c>
       <c r="O28" s="13"/>
-      <c r="P28" s="43" t="s">
+      <c r="P28" s="27" t="s">
         <v>176</v>
       </c>
       <c r="Q28" t="s">
@@ -3164,27 +3164,27 @@
       <c r="U28" t="s">
         <v>7</v>
       </c>
-      <c r="V28" s="45"/>
-      <c r="W28" s="44" t="s">
+      <c r="V28" s="29"/>
+      <c r="W28" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="X28" s="45" t="s">
+      <c r="X28" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="Y28" s="45"/>
-      <c r="Z28" s="45" t="s">
+      <c r="Y28" s="29"/>
+      <c r="Z28" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="AB28" s="45" t="s">
+      <c r="AB28" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="AD28" s="45" t="s">
+      <c r="AD28" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="AH28" s="44" t="s">
+      <c r="AH28" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="AI28" s="45" t="s">
+      <c r="AI28" s="29" t="s">
         <v>40</v>
       </c>
       <c r="AJ28" t="s">
@@ -3198,20 +3198,20 @@
       <c r="F29" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="28"/>
-      <c r="H29" s="29"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="46"/>
       <c r="I29" s="8"/>
       <c r="J29" s="8"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="46"/>
-      <c r="N29" s="44" t="s">
+      <c r="M29" s="30"/>
+      <c r="N29" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="P29" s="43"/>
+      <c r="P29" s="27"/>
       <c r="Q29" t="s">
         <v>18</v>
       </c>
-      <c r="W29" s="44"/>
+      <c r="W29" s="28"/>
       <c r="X29" t="s">
         <v>48</v>
       </c>
@@ -3224,7 +3224,7 @@
       <c r="AD29" t="s">
         <v>3</v>
       </c>
-      <c r="AH29" s="44"/>
+      <c r="AH29" s="28"/>
       <c r="AI29" t="s">
         <v>3</v>
       </c>
@@ -3233,24 +3233,24 @@
       </c>
     </row>
     <row r="30" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="49" t="s">
+      <c r="E30" s="33" t="s">
         <v>101</v>
       </c>
       <c r="F30" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="G30" s="28"/>
-      <c r="H30" s="29"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="46"/>
       <c r="L30" s="1"/>
-      <c r="M30" s="46"/>
-      <c r="N30" s="47" t="s">
+      <c r="M30" s="30"/>
+      <c r="N30" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="P30" s="43"/>
+      <c r="P30" s="27"/>
       <c r="Q30" t="s">
         <v>8</v>
       </c>
-      <c r="W30" s="44"/>
+      <c r="W30" s="28"/>
       <c r="X30" t="s">
         <v>54</v>
       </c>
@@ -3263,7 +3263,7 @@
       <c r="AD30" t="s">
         <v>13</v>
       </c>
-      <c r="AH30" s="44"/>
+      <c r="AH30" s="28"/>
       <c r="AI30" t="s">
         <v>13</v>
       </c>
@@ -3272,11 +3272,11 @@
       </c>
     </row>
     <row r="31" spans="1:48" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G31" s="28"/>
-      <c r="H31" s="29"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="46"/>
       <c r="L31" s="1"/>
       <c r="M31" s="13"/>
-      <c r="W31" s="44"/>
+      <c r="W31" s="28"/>
       <c r="X31" t="s">
         <v>58</v>
       </c>
@@ -3289,7 +3289,7 @@
       <c r="AD31" t="s">
         <v>23</v>
       </c>
-      <c r="AH31" s="44"/>
+      <c r="AH31" s="28"/>
       <c r="AI31" t="s">
         <v>23</v>
       </c>
@@ -3298,16 +3298,16 @@
       </c>
     </row>
     <row r="32" spans="1:48" x14ac:dyDescent="0.2">
-      <c r="G32" s="28"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="35" t="s">
+      <c r="G32" s="45"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="52" t="s">
         <v>97</v>
       </c>
-      <c r="J32" s="37"/>
-      <c r="K32" s="36"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="53"/>
       <c r="L32" s="1"/>
       <c r="M32" s="13"/>
-      <c r="P32" s="44" t="s">
+      <c r="P32" s="28" t="s">
         <v>177</v>
       </c>
       <c r="Q32" t="s">
@@ -3319,7 +3319,7 @@
       <c r="U32" t="s">
         <v>17</v>
       </c>
-      <c r="W32" s="44"/>
+      <c r="W32" s="28"/>
       <c r="X32" t="s">
         <v>34</v>
       </c>
@@ -3332,7 +3332,7 @@
       <c r="AD32" t="s">
         <v>33</v>
       </c>
-      <c r="AH32" s="44"/>
+      <c r="AH32" s="28"/>
       <c r="AI32" t="s">
         <v>33</v>
       </c>
@@ -3341,26 +3341,26 @@
       </c>
     </row>
     <row r="33" spans="2:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G33" s="28"/>
-      <c r="H33" s="30"/>
+      <c r="G33" s="45"/>
+      <c r="H33" s="47"/>
       <c r="I33" s="25" t="s">
         <v>63</v>
       </c>
       <c r="J33" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="K33" s="51" t="s">
+      <c r="K33" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="P33" s="44"/>
+      <c r="P33" s="28"/>
       <c r="Q33" t="s">
         <v>36</v>
       </c>
-      <c r="W33" s="44"/>
+      <c r="W33" s="28"/>
       <c r="X33" t="s">
         <v>42</v>
       </c>
-      <c r="Z33" s="45" t="s">
+      <c r="Z33" s="29" t="s">
         <v>7</v>
       </c>
       <c r="AB33" t="s">
@@ -3369,31 +3369,31 @@
       <c r="AD33" t="s">
         <v>41</v>
       </c>
-      <c r="AH33" s="44"/>
+      <c r="AH33" s="28"/>
       <c r="AI33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="34" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="D34" s="26" t="s">
+      <c r="D34" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="E34" s="33"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="30"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="47"/>
       <c r="I34" s="25" t="s">
         <v>77</v>
       </c>
       <c r="J34" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="K34" s="51"/>
-      <c r="P34" s="44"/>
+      <c r="K34" s="55"/>
+      <c r="P34" s="28"/>
       <c r="Q34" t="s">
         <v>28</v>
       </c>
-      <c r="W34" s="44"/>
+      <c r="W34" s="28"/>
       <c r="X34" t="s">
         <v>35</v>
       </c>
@@ -3406,86 +3406,89 @@
       <c r="AD34" t="s">
         <v>49</v>
       </c>
-      <c r="AH34" s="44"/>
+      <c r="AH34" s="28"/>
       <c r="AI34" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="35" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B35" s="1"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="29"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="30"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="47"/>
       <c r="I35" s="25" t="s">
         <v>68</v>
       </c>
       <c r="J35" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="K35" s="51"/>
-      <c r="W35" s="44"/>
+      <c r="K35" s="55"/>
+      <c r="W35" s="28"/>
       <c r="X35" t="s">
         <v>43</v>
       </c>
       <c r="Z35" t="s">
         <v>27</v>
       </c>
-      <c r="AH35" s="44"/>
+      <c r="AH35" s="28"/>
       <c r="AI35" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="36" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B36" s="1"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="29"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="30"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="47"/>
       <c r="I36" s="6"/>
       <c r="J36" s="8"/>
-      <c r="K36" s="51"/>
-      <c r="P36" s="44" t="s">
+      <c r="K36" s="55"/>
+      <c r="P36" s="28" t="s">
         <v>178</v>
       </c>
       <c r="Q36" t="s">
         <v>39</v>
       </c>
-      <c r="W36" s="44"/>
+      <c r="U36" t="s">
+        <v>48</v>
+      </c>
+      <c r="W36" s="28"/>
       <c r="X36" t="s">
-        <v>6</v>
-      </c>
-      <c r="AH36" s="44"/>
+        <v>190</v>
+      </c>
+      <c r="AH36" s="28"/>
     </row>
     <row r="37" spans="2:39" x14ac:dyDescent="0.2">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="53" t="s">
+      <c r="D37" s="45"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="36" t="s">
         <v>99</v>
       </c>
       <c r="J37" s="8"/>
-      <c r="K37" s="52" t="s">
+      <c r="K37" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="P37" s="44"/>
+      <c r="P37" s="28"/>
       <c r="Q37" t="s">
         <v>2</v>
       </c>
-      <c r="W37" s="44"/>
+      <c r="W37" s="28"/>
       <c r="X37" t="s">
         <v>16</v>
       </c>
-      <c r="AH37" s="44" t="s">
+      <c r="AH37" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="AK37" s="45" t="s">
+      <c r="AK37" s="29" t="s">
         <v>40</v>
       </c>
       <c r="AL37" t="s">
@@ -3493,27 +3496,27 @@
       </c>
     </row>
     <row r="38" spans="2:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D38" s="28"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="54" t="s">
+      <c r="D38" s="45"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="J38" s="55" t="s">
+      <c r="J38" s="38" t="s">
         <v>111</v>
       </c>
       <c r="K38" s="7"/>
-      <c r="P38" s="44"/>
+      <c r="P38" s="28"/>
       <c r="Q38" t="s">
         <v>4</v>
       </c>
-      <c r="W38" s="44"/>
+      <c r="W38" s="28"/>
       <c r="X38" t="s">
         <v>26</v>
       </c>
-      <c r="AH38" s="44"/>
+      <c r="AH38" s="28"/>
       <c r="AK38" t="s">
         <v>3</v>
       </c>
@@ -3522,20 +3525,20 @@
       </c>
     </row>
     <row r="39" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="D39" s="28"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="29"/>
-      <c r="P39" s="44"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="46"/>
+      <c r="P39" s="28"/>
       <c r="Q39" t="s">
         <v>5</v>
       </c>
-      <c r="W39" s="44"/>
+      <c r="W39" s="28"/>
       <c r="X39" t="s">
         <v>7</v>
       </c>
-      <c r="AH39" s="44"/>
+      <c r="AH39" s="28"/>
       <c r="AK39" t="s">
         <v>13</v>
       </c>
@@ -3544,20 +3547,20 @@
       </c>
     </row>
     <row r="40" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="D40" s="28"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="28"/>
-      <c r="H40" s="29"/>
-      <c r="P40" s="44"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="46"/>
+      <c r="P40" s="28"/>
       <c r="Q40" t="s">
         <v>44</v>
       </c>
-      <c r="W40" s="44"/>
+      <c r="W40" s="28"/>
       <c r="X40" t="s">
         <v>17</v>
       </c>
-      <c r="AH40" s="44"/>
+      <c r="AH40" s="28"/>
       <c r="AK40" t="s">
         <v>23</v>
       </c>
@@ -3566,20 +3569,20 @@
       </c>
     </row>
     <row r="41" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="D41" s="28"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="29"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="29"/>
-      <c r="P41" s="44"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="46"/>
+      <c r="P41" s="28"/>
       <c r="Q41" t="s">
         <v>28</v>
       </c>
-      <c r="W41" s="44"/>
+      <c r="W41" s="28"/>
       <c r="X41" t="s">
         <v>27</v>
       </c>
-      <c r="AH41" s="44"/>
+      <c r="AH41" s="28"/>
       <c r="AK41" t="s">
         <v>33</v>
       </c>
@@ -3597,95 +3600,95 @@
       <c r="F42" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="G42" s="28"/>
-      <c r="H42" s="29"/>
-      <c r="P42" s="44"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="46"/>
+      <c r="P42" s="28"/>
       <c r="Q42" t="s">
         <v>9</v>
       </c>
-      <c r="W42" s="44"/>
+      <c r="W42" s="28"/>
       <c r="X42" t="s">
         <v>37</v>
       </c>
-      <c r="AH42" s="44"/>
+      <c r="AH42" s="28"/>
       <c r="AK42" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="43" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="G43" s="28"/>
-      <c r="H43" s="29"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="46"/>
       <c r="I43" s="9" t="s">
         <v>93</v>
       </c>
       <c r="J43" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="P43" s="44"/>
+      <c r="P43" s="28"/>
       <c r="Q43" t="s">
         <v>45</v>
       </c>
-      <c r="W43" s="44"/>
+      <c r="W43" s="28"/>
       <c r="X43" t="s">
         <v>60</v>
       </c>
-      <c r="AH43" s="44"/>
+      <c r="AH43" s="28"/>
       <c r="AK43" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="44" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="G44" s="28"/>
-      <c r="H44" s="29"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="46"/>
       <c r="I44" s="21" t="s">
         <v>95</v>
       </c>
       <c r="J44" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="P44" s="44"/>
+      <c r="P44" s="28"/>
       <c r="Q44" t="s">
         <v>10</v>
       </c>
-      <c r="W44" s="44"/>
+      <c r="W44" s="28"/>
       <c r="X44" t="s">
         <v>38</v>
       </c>
-      <c r="AH44" s="44"/>
+      <c r="AH44" s="28"/>
       <c r="AK44" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="45" spans="2:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G45" s="28"/>
-      <c r="H45" s="29"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="46"/>
       <c r="I45" s="23" t="s">
         <v>6</v>
       </c>
       <c r="J45" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="P45" s="44"/>
+      <c r="P45" s="28"/>
       <c r="Q45" t="s">
         <v>46</v>
       </c>
-      <c r="W45" s="44"/>
+      <c r="W45" s="28"/>
       <c r="X45" t="s">
         <v>61</v>
       </c>
-      <c r="AH45" s="44"/>
+      <c r="AH45" s="28"/>
     </row>
     <row r="46" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="G46" s="28"/>
-      <c r="H46" s="29"/>
-      <c r="W46" s="44"/>
-      <c r="AH46" s="44" t="s">
+      <c r="G46" s="45"/>
+      <c r="H46" s="46"/>
+      <c r="W46" s="28"/>
+      <c r="AH46" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="AJ46" s="48" t="s">
+      <c r="AJ46" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="AL46" s="45" t="s">
+      <c r="AL46" s="29" t="s">
         <v>40</v>
       </c>
       <c r="AM46" t="s">
@@ -3693,30 +3696,33 @@
       </c>
     </row>
     <row r="47" spans="2:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G47" s="28"/>
-      <c r="H47" s="29"/>
-      <c r="P47" s="44" t="s">
+      <c r="G47" s="45"/>
+      <c r="H47" s="46"/>
+      <c r="P47" s="28" t="s">
         <v>179</v>
       </c>
       <c r="Q47" t="s">
         <v>47</v>
       </c>
-      <c r="W47" s="44" t="s">
+      <c r="U47" t="s">
+        <v>54</v>
+      </c>
+      <c r="W47" s="28" t="s">
         <v>181</v>
       </c>
-      <c r="Y47" s="45" t="s">
+      <c r="Y47" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="AA47" s="45" t="s">
+      <c r="AA47" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="AC47" s="45" t="s">
+      <c r="AC47" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="AE47" s="45" t="s">
+      <c r="AE47" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="AH47" s="44"/>
+      <c r="AH47" s="28"/>
       <c r="AJ47" t="s">
         <v>3</v>
       </c>
@@ -3728,16 +3734,16 @@
       </c>
     </row>
     <row r="48" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="G48" s="28"/>
-      <c r="H48" s="29"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="46"/>
       <c r="I48" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="P48" s="44"/>
+      <c r="P48" s="28"/>
       <c r="Q48" t="s">
         <v>12</v>
       </c>
-      <c r="W48" s="44"/>
+      <c r="W48" s="28"/>
       <c r="Y48" t="s">
         <v>48</v>
       </c>
@@ -3750,7 +3756,7 @@
       <c r="AE48" t="s">
         <v>3</v>
       </c>
-      <c r="AH48" s="44"/>
+      <c r="AH48" s="28"/>
       <c r="AJ48" t="s">
         <v>13</v>
       </c>
@@ -3762,16 +3768,16 @@
       </c>
     </row>
     <row r="49" spans="2:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G49" s="28"/>
-      <c r="H49" s="29"/>
-      <c r="I49" s="50" t="s">
+      <c r="G49" s="45"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="P49" s="44"/>
+      <c r="P49" s="28"/>
       <c r="Q49" t="s">
         <v>14</v>
       </c>
-      <c r="W49" s="44"/>
+      <c r="W49" s="28"/>
       <c r="Y49" t="s">
         <v>54</v>
       </c>
@@ -3784,7 +3790,7 @@
       <c r="AE49" t="s">
         <v>13</v>
       </c>
-      <c r="AH49" s="44"/>
+      <c r="AH49" s="28"/>
       <c r="AJ49" t="s">
         <v>23</v>
       </c>
@@ -3793,13 +3799,13 @@
       </c>
     </row>
     <row r="50" spans="2:40" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G50" s="31"/>
-      <c r="H50" s="32"/>
-      <c r="P50" s="44"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="49"/>
+      <c r="P50" s="28"/>
       <c r="Q50" t="s">
         <v>15</v>
       </c>
-      <c r="W50" s="44"/>
+      <c r="W50" s="28"/>
       <c r="Y50" t="s">
         <v>58</v>
       </c>
@@ -3812,7 +3818,7 @@
       <c r="AE50" t="s">
         <v>23</v>
       </c>
-      <c r="AH50" s="44"/>
+      <c r="AH50" s="28"/>
       <c r="AJ50" t="s">
         <v>33</v>
       </c>
@@ -3821,11 +3827,11 @@
       </c>
     </row>
     <row r="51" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="P51" s="44"/>
+      <c r="P51" s="28"/>
       <c r="Q51" t="s">
         <v>8</v>
       </c>
-      <c r="W51" s="44"/>
+      <c r="W51" s="28"/>
       <c r="Y51" t="s">
         <v>34</v>
       </c>
@@ -3838,7 +3844,7 @@
       <c r="AE51" t="s">
         <v>33</v>
       </c>
-      <c r="AH51" s="44"/>
+      <c r="AH51" s="28"/>
       <c r="AJ51" t="s">
         <v>41</v>
       </c>
@@ -3847,15 +3853,15 @@
       </c>
     </row>
     <row r="52" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="P52" s="44"/>
+      <c r="P52" s="28"/>
       <c r="Q52" t="s">
         <v>50</v>
       </c>
-      <c r="W52" s="44"/>
+      <c r="W52" s="28"/>
       <c r="Y52" t="s">
         <v>42</v>
       </c>
-      <c r="AA52" s="45" t="s">
+      <c r="AA52" s="29" t="s">
         <v>7</v>
       </c>
       <c r="AC52" t="s">
@@ -3864,7 +3870,7 @@
       <c r="AE52" t="s">
         <v>41</v>
       </c>
-      <c r="AH52" s="44"/>
+      <c r="AH52" s="28"/>
       <c r="AJ52" t="s">
         <v>49</v>
       </c>
@@ -3873,11 +3879,11 @@
       </c>
     </row>
     <row r="53" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="P53" s="44"/>
+      <c r="P53" s="28"/>
       <c r="Q53" t="s">
         <v>19</v>
       </c>
-      <c r="W53" s="44"/>
+      <c r="W53" s="28"/>
       <c r="Y53" t="s">
         <v>35</v>
       </c>
@@ -3890,72 +3896,72 @@
       <c r="AE53" t="s">
         <v>49</v>
       </c>
-      <c r="AH53" s="44"/>
+      <c r="AH53" s="28"/>
     </row>
     <row r="54" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B54" s="44" t="s">
+      <c r="B54" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="42" t="s">
+      <c r="C54" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="D54" s="42" t="s">
+      <c r="D54" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="E54" s="42" t="s">
+      <c r="E54" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="F54" s="42" t="s">
+      <c r="F54" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="G54" s="42" t="s">
+      <c r="G54" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="H54" s="42" t="s">
+      <c r="H54" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="I54" s="42" t="s">
+      <c r="I54" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="J54" s="42" t="s">
+      <c r="J54" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="K54" s="42" t="s">
+      <c r="K54" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="P54" s="44"/>
+      <c r="P54" s="28"/>
       <c r="Q54" t="s">
         <v>51</v>
       </c>
-      <c r="W54" s="44"/>
+      <c r="W54" s="28"/>
       <c r="Y54" t="s">
         <v>43</v>
       </c>
       <c r="AA54" t="s">
         <v>27</v>
       </c>
-      <c r="AH54" s="44"/>
-      <c r="AI54" s="42" t="s">
+      <c r="AH54" s="28"/>
+      <c r="AI54" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="AJ54" s="42" t="s">
+      <c r="AJ54" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="AK54" s="42" t="s">
+      <c r="AK54" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="AL54" s="42" t="s">
+      <c r="AL54" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="AM54" s="42" t="s">
+      <c r="AM54" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="AN54" s="42" t="s">
+      <c r="AN54" s="26" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="55" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B55" s="44" t="s">
+      <c r="B55" s="28" t="s">
         <v>63</v>
       </c>
       <c r="C55" t="s">
@@ -3967,15 +3973,15 @@
       <c r="G55" t="s">
         <v>34</v>
       </c>
-      <c r="P55" s="44"/>
+      <c r="P55" s="28"/>
       <c r="Q55" t="s">
         <v>20</v>
       </c>
-      <c r="W55" s="44"/>
+      <c r="W55" s="28"/>
       <c r="Y55" t="s">
         <v>6</v>
       </c>
-      <c r="AH55" s="44" t="s">
+      <c r="AH55" s="28" t="s">
         <v>102</v>
       </c>
       <c r="AJ55" t="s">
@@ -3989,46 +3995,46 @@
       </c>
     </row>
     <row r="56" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B56" s="44"/>
+      <c r="B56" s="28"/>
       <c r="C56" t="s">
         <v>14</v>
       </c>
-      <c r="P56" s="44"/>
+      <c r="P56" s="28"/>
       <c r="Q56" t="s">
         <v>52</v>
       </c>
-      <c r="W56" s="44"/>
+      <c r="W56" s="28"/>
       <c r="Y56" t="s">
         <v>16</v>
       </c>
-      <c r="AH56" s="44"/>
+      <c r="AH56" s="28"/>
       <c r="AM56" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="57" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B57" s="44"/>
+      <c r="B57" s="28"/>
       <c r="C57" t="s">
         <v>24</v>
       </c>
-      <c r="W57" s="44"/>
+      <c r="W57" s="28"/>
       <c r="Y57" t="s">
         <v>26</v>
       </c>
-      <c r="AH57" s="44"/>
+      <c r="AH57" s="28"/>
       <c r="AM57" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="58" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B58" s="44"/>
-      <c r="W58" s="44"/>
+      <c r="B58" s="28"/>
+      <c r="W58" s="28"/>
       <c r="Y58" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="59" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B59" s="44" t="s">
+      <c r="B59" s="28" t="s">
         <v>64</v>
       </c>
       <c r="C59" t="s">
@@ -4040,40 +4046,40 @@
       <c r="G59" t="s">
         <v>35</v>
       </c>
-      <c r="W59" s="44"/>
+      <c r="W59" s="28"/>
       <c r="Y59" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="60" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B60" s="44"/>
+      <c r="B60" s="28"/>
       <c r="C60" t="s">
         <v>15</v>
       </c>
-      <c r="W60" s="44"/>
+      <c r="W60" s="28"/>
       <c r="Y60" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="61" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B61" s="44"/>
+      <c r="B61" s="28"/>
       <c r="C61" t="s">
         <v>25</v>
       </c>
-      <c r="W61" s="44"/>
+      <c r="W61" s="28"/>
       <c r="Y61" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="62" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B62" s="44"/>
-      <c r="W62" s="44"/>
+      <c r="B62" s="28"/>
+      <c r="W62" s="28"/>
       <c r="Y62" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="63" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B63" s="44" t="s">
+      <c r="B63" s="28" t="s">
         <v>77</v>
       </c>
       <c r="C63" t="s">
@@ -4082,36 +4088,36 @@
       <c r="D63" t="s">
         <v>37</v>
       </c>
-      <c r="W63" s="44"/>
+      <c r="W63" s="28"/>
       <c r="Y63" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="64" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B64" s="44"/>
+      <c r="B64" s="28"/>
       <c r="C64" t="s">
         <v>19</v>
       </c>
-      <c r="W64" s="44"/>
+      <c r="W64" s="28"/>
       <c r="Y64" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="65" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B65" s="44"/>
-      <c r="W65" s="44"/>
+      <c r="B65" s="28"/>
+      <c r="W65" s="28"/>
     </row>
     <row r="66" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B66" s="44"/>
-      <c r="W66" s="44" t="s">
+      <c r="B66" s="28"/>
+      <c r="W66" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="Y66" s="45" t="s">
+      <c r="Y66" s="29" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="67" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B67" s="44" t="s">
+      <c r="B67" s="28" t="s">
         <v>72</v>
       </c>
       <c r="C67" t="s">
@@ -4120,30 +4126,30 @@
       <c r="D67" t="s">
         <v>60</v>
       </c>
-      <c r="W67" s="44"/>
+      <c r="W67" s="28"/>
       <c r="Y67" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="68" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B68" s="44"/>
+      <c r="B68" s="28"/>
       <c r="C68" t="s">
         <v>51</v>
       </c>
-      <c r="W68" s="44"/>
+      <c r="W68" s="28"/>
       <c r="Y68" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="69" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B69" s="44"/>
-      <c r="W69" s="44"/>
+      <c r="B69" s="28"/>
+      <c r="W69" s="28"/>
       <c r="Y69" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="70" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B70" s="44" t="s">
+      <c r="B70" s="28" t="s">
         <v>68</v>
       </c>
       <c r="C70" t="s">
@@ -4152,64 +4158,61 @@
       <c r="D70" t="s">
         <v>38</v>
       </c>
-      <c r="W70" s="44"/>
+      <c r="W70" s="28"/>
       <c r="Y70" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="71" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B71" s="44"/>
+      <c r="B71" s="28"/>
       <c r="C71" t="s">
         <v>20</v>
       </c>
-      <c r="W71" s="44"/>
+      <c r="W71" s="28"/>
       <c r="Y71" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="72" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B72" s="44"/>
-      <c r="C72" t="s">
-        <v>30</v>
-      </c>
-      <c r="W72" s="44"/>
+      <c r="B72" s="28"/>
+      <c r="W72" s="28"/>
       <c r="Y72" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="73" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B73" s="44"/>
-      <c r="W73" s="44"/>
-      <c r="X73" s="42" t="s">
+      <c r="B73" s="28"/>
+      <c r="W73" s="28"/>
+      <c r="X73" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="Y73" s="42" t="s">
+      <c r="Y73" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="Z73" s="42" t="s">
+      <c r="Z73" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="AA73" s="42" t="s">
+      <c r="AA73" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="AB73" s="42" t="s">
+      <c r="AB73" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="AC73" s="42" t="s">
+      <c r="AC73" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="AD73" s="42" t="s">
+      <c r="AD73" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="AE73" s="42" t="s">
+      <c r="AE73" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="AF73" s="42" t="s">
+      <c r="AF73" s="26" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="74" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B74" s="44" t="s">
+      <c r="B74" s="28" t="s">
         <v>73</v>
       </c>
       <c r="C74" t="s">
@@ -4218,991 +4221,1073 @@
       <c r="D74" t="s">
         <v>61</v>
       </c>
-      <c r="W74" s="44" t="s">
+      <c r="W74" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="AA74" s="45" t="s">
+      <c r="AA74" s="29" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="75" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B75" s="44"/>
+      <c r="B75" s="28"/>
       <c r="C75" t="s">
         <v>52</v>
       </c>
-      <c r="W75" s="44"/>
+      <c r="W75" s="28"/>
       <c r="AA75" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="76" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B76" s="44"/>
+      <c r="B76" s="28"/>
       <c r="C76" t="s">
         <v>57</v>
       </c>
-      <c r="W76" s="44"/>
+      <c r="W76" s="28"/>
       <c r="AA76" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="77" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B77" s="44"/>
-      <c r="W77" s="44"/>
+      <c r="B77" s="28"/>
+      <c r="W77" s="28"/>
       <c r="AA77" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="78" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B78" s="44" t="s">
-        <v>188</v>
+      <c r="B78" s="28" t="s">
+        <v>98</v>
       </c>
       <c r="C78" t="s">
         <v>4</v>
       </c>
       <c r="D78" t="s">
-        <v>4</v>
-      </c>
-      <c r="W78" s="44"/>
+        <v>42</v>
+      </c>
+      <c r="G78" t="s">
+        <v>34</v>
+      </c>
+      <c r="W78" s="28"/>
       <c r="AA78" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="79" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B79" s="44"/>
+      <c r="B79" s="28"/>
       <c r="C79" t="s">
         <v>14</v>
       </c>
       <c r="D79" t="s">
-        <v>14</v>
-      </c>
-      <c r="W79" s="44"/>
+        <v>43</v>
+      </c>
+      <c r="G79" t="s">
+        <v>35</v>
+      </c>
+      <c r="W79" s="28"/>
       <c r="AA79" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="80" spans="2:32" x14ac:dyDescent="0.2">
-      <c r="B80" s="44"/>
+      <c r="B80" s="28"/>
       <c r="C80" t="s">
         <v>24</v>
       </c>
       <c r="D80" t="s">
-        <v>24</v>
-      </c>
-      <c r="W80" s="44"/>
+        <v>37</v>
+      </c>
+      <c r="W80" s="28"/>
       <c r="AA80" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="81" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B81" s="44"/>
+      <c r="B81" s="28"/>
       <c r="C81" t="s">
         <v>5</v>
       </c>
       <c r="D81" t="s">
-        <v>5</v>
-      </c>
-      <c r="W81" s="44"/>
+        <v>60</v>
+      </c>
+      <c r="W81" s="28"/>
     </row>
     <row r="82" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B82" s="44"/>
+      <c r="B82" s="28"/>
       <c r="C82" t="s">
         <v>15</v>
       </c>
       <c r="D82" t="s">
-        <v>15</v>
-      </c>
-      <c r="W82" s="44" t="s">
+        <v>38</v>
+      </c>
+      <c r="W82" s="28" t="s">
         <v>184</v>
       </c>
       <c r="Y82" t="s">
         <v>55</v>
       </c>
-      <c r="AC82" s="45" t="s">
+      <c r="AC82" s="29" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="83" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B83" s="44"/>
+      <c r="B83" s="28"/>
       <c r="C83" t="s">
         <v>25</v>
       </c>
       <c r="D83" t="s">
-        <v>25</v>
-      </c>
-      <c r="W83" s="44"/>
+        <v>61</v>
+      </c>
+      <c r="W83" s="28"/>
       <c r="AC83" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="84" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B84" s="44"/>
+      <c r="B84" s="28"/>
       <c r="C84" t="s">
         <v>9</v>
       </c>
-      <c r="D84" t="s">
-        <v>9</v>
-      </c>
-      <c r="W84" s="44"/>
+      <c r="W84" s="28"/>
       <c r="AC84" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="85" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B85" s="44"/>
+      <c r="B85" s="28"/>
       <c r="C85" t="s">
         <v>19</v>
       </c>
-      <c r="D85" t="s">
-        <v>19</v>
-      </c>
-      <c r="W85" s="44"/>
+      <c r="W85" s="28"/>
       <c r="AC85" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="86" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B86" s="44"/>
+      <c r="B86" s="28"/>
       <c r="C86" t="s">
         <v>45</v>
       </c>
-      <c r="D86" t="s">
-        <v>45</v>
-      </c>
-      <c r="W86" s="44"/>
+      <c r="W86" s="28"/>
       <c r="AC86" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="87" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B87" s="44"/>
+      <c r="B87" s="28"/>
       <c r="C87" t="s">
         <v>51</v>
       </c>
-      <c r="D87" t="s">
-        <v>51</v>
-      </c>
-      <c r="W87" s="44"/>
+      <c r="W87" s="28"/>
       <c r="AC87" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="88" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B88" s="44"/>
+      <c r="B88" s="28"/>
       <c r="C88" t="s">
         <v>10</v>
       </c>
-      <c r="D88" t="s">
-        <v>10</v>
-      </c>
-      <c r="W88" s="44"/>
+      <c r="W88" s="28"/>
       <c r="AC88" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="89" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B89" s="44"/>
+      <c r="B89" s="28"/>
       <c r="C89" t="s">
         <v>20</v>
       </c>
-      <c r="D89" t="s">
-        <v>20</v>
-      </c>
-      <c r="W89" s="44"/>
+      <c r="W89" s="28"/>
     </row>
     <row r="90" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B90" s="44"/>
+      <c r="B90" s="28"/>
       <c r="C90" t="s">
-        <v>30</v>
-      </c>
-      <c r="D90" t="s">
-        <v>30</v>
-      </c>
-      <c r="W90" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="W90" s="28" t="s">
         <v>185</v>
       </c>
       <c r="AA90" t="s">
         <v>55</v>
       </c>
-      <c r="AE90" s="45" t="s">
+      <c r="AE90" s="29" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="91" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B91" s="44"/>
+      <c r="B91" s="28"/>
       <c r="C91" t="s">
-        <v>46</v>
-      </c>
-      <c r="D91" t="s">
-        <v>46</v>
-      </c>
-      <c r="W91" s="44"/>
+        <v>52</v>
+      </c>
+      <c r="W91" s="28"/>
       <c r="AE91" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="92" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B92" s="44"/>
+      <c r="B92" s="28"/>
       <c r="C92" t="s">
-        <v>52</v>
-      </c>
-      <c r="D92" t="s">
-        <v>52</v>
-      </c>
-      <c r="W92" s="44"/>
+        <v>57</v>
+      </c>
+      <c r="W92" s="28"/>
       <c r="AE92" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="93" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B93" s="44"/>
-      <c r="C93" t="s">
-        <v>57</v>
-      </c>
-      <c r="D93" t="s">
-        <v>57</v>
-      </c>
-      <c r="W93" s="44"/>
+      <c r="B93" s="28"/>
+      <c r="W93" s="28"/>
       <c r="AE93" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="94" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B94" s="44"/>
-      <c r="W94" s="44"/>
+      <c r="B94" s="28"/>
+      <c r="W94" s="28"/>
       <c r="AE94" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="95" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B95" s="44" t="s">
-        <v>99</v>
-      </c>
-      <c r="C95" t="s">
-        <v>2</v>
+      <c r="B95" t="s">
+        <v>112</v>
       </c>
       <c r="D95" t="s">
-        <v>78</v>
-      </c>
-      <c r="W95" s="44"/>
+        <v>4</v>
+      </c>
+      <c r="E95" t="s">
+        <v>42</v>
+      </c>
+      <c r="H95" t="s">
+        <v>34</v>
+      </c>
+      <c r="W95" s="28"/>
       <c r="AE95" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="96" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B96" s="44"/>
-      <c r="C96" t="s">
-        <v>12</v>
-      </c>
-      <c r="W96" s="44"/>
+      <c r="D96" t="s">
+        <v>14</v>
+      </c>
+      <c r="E96" t="s">
+        <v>43</v>
+      </c>
+      <c r="H96" t="s">
+        <v>35</v>
+      </c>
+      <c r="W96" s="28"/>
       <c r="AE96" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="97" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B97" s="44"/>
-      <c r="W97" s="44"/>
-    </row>
-    <row r="98" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B98" s="44" t="s">
+    <row r="97" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D97" t="s">
+        <v>24</v>
+      </c>
+      <c r="E97" t="s">
+        <v>37</v>
+      </c>
+      <c r="W97" s="28"/>
+    </row>
+    <row r="98" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D98" t="s">
+        <v>5</v>
+      </c>
+      <c r="E98" t="s">
+        <v>60</v>
+      </c>
+      <c r="W98" s="28"/>
+    </row>
+    <row r="99" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D99" t="s">
+        <v>15</v>
+      </c>
+      <c r="E99" t="s">
+        <v>38</v>
+      </c>
+      <c r="W99" s="28"/>
+    </row>
+    <row r="100" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
+        <v>25</v>
+      </c>
+      <c r="E100" t="s">
+        <v>61</v>
+      </c>
+      <c r="W100" s="28"/>
+    </row>
+    <row r="101" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D101" t="s">
+        <v>9</v>
+      </c>
+      <c r="W101" s="28"/>
+    </row>
+    <row r="102" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D102" t="s">
+        <v>19</v>
+      </c>
+      <c r="W102" s="28"/>
+    </row>
+    <row r="103" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D103" t="s">
+        <v>45</v>
+      </c>
+      <c r="W103" s="28"/>
+    </row>
+    <row r="104" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D104" t="s">
+        <v>51</v>
+      </c>
+      <c r="W104" s="28"/>
+    </row>
+    <row r="105" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D105" t="s">
+        <v>10</v>
+      </c>
+      <c r="W105" s="28"/>
+    </row>
+    <row r="106" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D106" t="s">
+        <v>20</v>
+      </c>
+      <c r="W106" s="28"/>
+    </row>
+    <row r="107" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D107" t="s">
+        <v>30</v>
+      </c>
+      <c r="W107" s="28"/>
+    </row>
+    <row r="108" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D108" t="s">
+        <v>46</v>
+      </c>
+      <c r="W108" s="28"/>
+    </row>
+    <row r="109" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D109" t="s">
+        <v>52</v>
+      </c>
+      <c r="W109" s="28"/>
+    </row>
+    <row r="110" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D110" t="s">
+        <v>57</v>
+      </c>
+      <c r="W110" s="28"/>
+    </row>
+    <row r="111" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="W111" s="28"/>
+    </row>
+    <row r="112" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="W112" s="28"/>
+    </row>
+    <row r="113" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="W113" s="28"/>
+    </row>
+    <row r="114" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="W114" s="28"/>
+    </row>
+    <row r="115" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="W115" s="28"/>
+    </row>
+    <row r="116" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="W116" s="28"/>
+    </row>
+    <row r="117" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="W117" s="28"/>
+    </row>
+    <row r="118" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B118" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C118" t="s">
+        <v>2</v>
+      </c>
+      <c r="D118" t="s">
+        <v>78</v>
+      </c>
+      <c r="W118" s="28"/>
+    </row>
+    <row r="119" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B119" s="28"/>
+      <c r="C119" t="s">
+        <v>12</v>
+      </c>
+      <c r="W119" s="28"/>
+    </row>
+    <row r="120" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B120" s="28"/>
+      <c r="W120" s="28"/>
+    </row>
+    <row r="121" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B121" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="C121" t="s">
+        <v>31</v>
+      </c>
+      <c r="D121" t="s">
+        <v>26</v>
+      </c>
+      <c r="E121" t="s">
+        <v>42</v>
+      </c>
+      <c r="G121" t="s">
+        <v>27</v>
+      </c>
+      <c r="H121" t="s">
+        <v>34</v>
+      </c>
+      <c r="W121" s="28"/>
+    </row>
+    <row r="122" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B122" s="28"/>
+      <c r="D122" t="s">
+        <v>4</v>
+      </c>
+      <c r="E122" t="s">
+        <v>43</v>
+      </c>
+      <c r="H122" t="s">
+        <v>35</v>
+      </c>
+      <c r="W122" s="28"/>
+    </row>
+    <row r="123" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B123" s="28"/>
+      <c r="D123" t="s">
+        <v>14</v>
+      </c>
+      <c r="E123" t="s">
+        <v>37</v>
+      </c>
+      <c r="W123" s="28"/>
+    </row>
+    <row r="124" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B124" s="28"/>
+      <c r="D124" t="s">
+        <v>24</v>
+      </c>
+      <c r="E124" t="s">
+        <v>60</v>
+      </c>
+      <c r="W124" s="28"/>
+    </row>
+    <row r="125" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B125" s="28"/>
+      <c r="D125" t="s">
+        <v>5</v>
+      </c>
+      <c r="E125" t="s">
+        <v>38</v>
+      </c>
+      <c r="W125" s="28"/>
+    </row>
+    <row r="126" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B126" s="28"/>
+      <c r="D126" t="s">
+        <v>15</v>
+      </c>
+      <c r="E126" t="s">
+        <v>61</v>
+      </c>
+      <c r="W126" s="28"/>
+    </row>
+    <row r="127" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B127" s="28"/>
+      <c r="D127" t="s">
+        <v>25</v>
+      </c>
+      <c r="W127" s="28"/>
+    </row>
+    <row r="128" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B128" s="28"/>
+      <c r="D128" t="s">
+        <v>9</v>
+      </c>
+      <c r="W128" s="28"/>
+    </row>
+    <row r="129" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B129" s="28"/>
+      <c r="D129" t="s">
+        <v>19</v>
+      </c>
+      <c r="W129" s="28"/>
+    </row>
+    <row r="130" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B130" s="28"/>
+      <c r="D130" t="s">
+        <v>45</v>
+      </c>
+      <c r="W130" s="28"/>
+    </row>
+    <row r="131" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B131" s="28"/>
+      <c r="D131" t="s">
+        <v>51</v>
+      </c>
+      <c r="W131" s="28"/>
+    </row>
+    <row r="132" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B132" s="28"/>
+      <c r="D132" t="s">
+        <v>10</v>
+      </c>
+      <c r="W132" s="28"/>
+    </row>
+    <row r="133" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B133" s="28"/>
+      <c r="D133" t="s">
+        <v>20</v>
+      </c>
+      <c r="W133" s="28"/>
+    </row>
+    <row r="134" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B134" s="28"/>
+      <c r="D134" t="s">
+        <v>30</v>
+      </c>
+      <c r="W134" s="28"/>
+    </row>
+    <row r="135" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B135" s="28"/>
+      <c r="D135" t="s">
+        <v>46</v>
+      </c>
+      <c r="W135" s="28"/>
+    </row>
+    <row r="136" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B136" s="28"/>
+      <c r="D136" t="s">
+        <v>52</v>
+      </c>
+      <c r="W136" s="28"/>
+    </row>
+    <row r="137" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B137" s="28"/>
+      <c r="D137" t="s">
+        <v>57</v>
+      </c>
+      <c r="W137" s="28"/>
+    </row>
+    <row r="138" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B138" s="28"/>
+      <c r="W138" s="28"/>
+    </row>
+    <row r="139" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B139" s="28" t="s">
         <v>189</v>
       </c>
-      <c r="D98" t="s">
-        <v>26</v>
-      </c>
-      <c r="G98" t="s">
-        <v>27</v>
-      </c>
-      <c r="W98" s="44"/>
-    </row>
-    <row r="99" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B99" s="44"/>
-      <c r="D99" t="s">
-        <v>4</v>
-      </c>
-      <c r="W99" s="44"/>
-    </row>
-    <row r="100" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B100" s="44"/>
-      <c r="D100" t="s">
-        <v>14</v>
-      </c>
-      <c r="W100" s="44"/>
-    </row>
-    <row r="101" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B101" s="44"/>
-      <c r="D101" t="s">
+      <c r="C139" t="s">
         <v>24</v>
       </c>
-      <c r="W101" s="44"/>
-    </row>
-    <row r="102" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B102" s="44"/>
-      <c r="D102" t="s">
-        <v>5</v>
-      </c>
-      <c r="W102" s="44"/>
-    </row>
-    <row r="103" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B103" s="44"/>
-      <c r="D103" t="s">
-        <v>15</v>
-      </c>
-      <c r="W103" s="44"/>
-    </row>
-    <row r="104" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B104" s="44"/>
-      <c r="D104" t="s">
+      <c r="W139" s="28"/>
+    </row>
+    <row r="140" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B140" s="28"/>
+      <c r="C140" t="s">
         <v>25</v>
       </c>
-      <c r="W104" s="44"/>
-    </row>
-    <row r="105" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B105" s="44"/>
-      <c r="D105" t="s">
-        <v>9</v>
-      </c>
-      <c r="W105" s="44"/>
-    </row>
-    <row r="106" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B106" s="44"/>
-      <c r="D106" t="s">
-        <v>19</v>
-      </c>
-      <c r="W106" s="44"/>
-    </row>
-    <row r="107" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B107" s="44"/>
-      <c r="D107" t="s">
-        <v>45</v>
-      </c>
-      <c r="W107" s="44"/>
-    </row>
-    <row r="108" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B108" s="44"/>
-      <c r="D108" t="s">
-        <v>51</v>
-      </c>
-      <c r="W108" s="44"/>
-    </row>
-    <row r="109" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B109" s="44"/>
-      <c r="D109" t="s">
-        <v>10</v>
-      </c>
-      <c r="W109" s="44"/>
-    </row>
-    <row r="110" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B110" s="44"/>
-      <c r="D110" t="s">
-        <v>20</v>
-      </c>
-      <c r="W110" s="44"/>
-    </row>
-    <row r="111" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B111" s="44"/>
-      <c r="D111" t="s">
-        <v>30</v>
-      </c>
-      <c r="W111" s="44"/>
-    </row>
-    <row r="112" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B112" s="44"/>
-      <c r="D112" t="s">
-        <v>46</v>
-      </c>
-      <c r="W112" s="44"/>
-    </row>
-    <row r="113" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B113" s="44"/>
-      <c r="D113" t="s">
-        <v>52</v>
-      </c>
-      <c r="W113" s="44"/>
-    </row>
-    <row r="114" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B114" s="44"/>
-      <c r="D114" t="s">
+      <c r="W140" s="28"/>
+    </row>
+    <row r="141" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="W141" s="28"/>
+    </row>
+    <row r="142" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="C142" t="s">
         <v>57</v>
       </c>
-      <c r="W114" s="44"/>
-    </row>
-    <row r="115" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B115" s="44"/>
-      <c r="W115" s="44"/>
-    </row>
-    <row r="116" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B116" s="44" t="s">
-        <v>190</v>
-      </c>
-      <c r="C116" t="s">
-        <v>24</v>
-      </c>
-      <c r="W116" s="44"/>
-    </row>
-    <row r="117" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B117" s="44"/>
-      <c r="C117" t="s">
-        <v>25</v>
-      </c>
-      <c r="W117" s="44"/>
-    </row>
-    <row r="118" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="C118" t="s">
-        <v>30</v>
-      </c>
-      <c r="W118" s="44"/>
-    </row>
-    <row r="119" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="C119" t="s">
-        <v>57</v>
-      </c>
-      <c r="W119" s="44"/>
-    </row>
-    <row r="120" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="W120" s="44"/>
-    </row>
-    <row r="121" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="W121" s="44"/>
-    </row>
-    <row r="122" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="W122" s="44"/>
-    </row>
-    <row r="123" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="W123" s="44"/>
-    </row>
-    <row r="124" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="W124" s="44"/>
-    </row>
-    <row r="125" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="W125" s="44"/>
-    </row>
-    <row r="126" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="W126" s="44"/>
-    </row>
-    <row r="127" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="W127" s="44"/>
-    </row>
-    <row r="128" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="W128" s="44"/>
-    </row>
-    <row r="129" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W129" s="44"/>
-    </row>
-    <row r="130" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W130" s="44"/>
-    </row>
-    <row r="131" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W131" s="44"/>
-    </row>
-    <row r="132" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W132" s="44"/>
-    </row>
-    <row r="133" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W133" s="44"/>
-    </row>
-    <row r="134" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W134" s="44"/>
-    </row>
-    <row r="135" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W135" s="44"/>
-    </row>
-    <row r="136" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W136" s="44"/>
-    </row>
-    <row r="137" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W137" s="44"/>
-    </row>
-    <row r="138" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W138" s="44"/>
-    </row>
-    <row r="139" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W139" s="44"/>
-    </row>
-    <row r="140" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W140" s="44"/>
-    </row>
-    <row r="141" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W141" s="44"/>
-    </row>
-    <row r="142" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W142" s="44"/>
-    </row>
-    <row r="143" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W143" s="44"/>
-    </row>
-    <row r="144" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W144" s="44"/>
+      <c r="W142" s="28"/>
+    </row>
+    <row r="143" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="C143" t="s">
+        <v>53</v>
+      </c>
+      <c r="W143" s="28"/>
+    </row>
+    <row r="144" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="W144" s="28"/>
     </row>
     <row r="145" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W145" s="44"/>
+      <c r="W145" s="28"/>
     </row>
     <row r="146" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W146" s="44"/>
+      <c r="W146" s="28"/>
     </row>
     <row r="147" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W147" s="44"/>
+      <c r="W147" s="28"/>
     </row>
     <row r="148" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W148" s="44"/>
+      <c r="W148" s="28"/>
     </row>
     <row r="149" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W149" s="44"/>
+      <c r="W149" s="28"/>
     </row>
     <row r="150" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W150" s="44"/>
+      <c r="W150" s="28"/>
     </row>
     <row r="151" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W151" s="44"/>
+      <c r="W151" s="28"/>
     </row>
     <row r="152" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W152" s="44"/>
+      <c r="W152" s="28"/>
     </row>
     <row r="153" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W153" s="44"/>
+      <c r="W153" s="28"/>
     </row>
     <row r="154" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W154" s="44"/>
+      <c r="W154" s="28"/>
     </row>
     <row r="155" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W155" s="44"/>
+      <c r="W155" s="28"/>
     </row>
     <row r="156" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W156" s="44"/>
+      <c r="W156" s="28"/>
     </row>
     <row r="157" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W157" s="44"/>
+      <c r="W157" s="28"/>
     </row>
     <row r="158" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W158" s="44"/>
+      <c r="W158" s="28"/>
     </row>
     <row r="159" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W159" s="44"/>
+      <c r="W159" s="28"/>
     </row>
     <row r="160" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W160" s="44"/>
+      <c r="W160" s="28"/>
     </row>
     <row r="161" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W161" s="44"/>
+      <c r="W161" s="28"/>
     </row>
     <row r="162" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W162" s="44"/>
+      <c r="W162" s="28"/>
     </row>
     <row r="163" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W163" s="44"/>
+      <c r="W163" s="28"/>
     </row>
     <row r="164" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W164" s="44"/>
+      <c r="W164" s="28"/>
     </row>
     <row r="165" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W165" s="44"/>
+      <c r="W165" s="28"/>
     </row>
     <row r="166" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W166" s="44"/>
+      <c r="W166" s="28"/>
     </row>
     <row r="167" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W167" s="44"/>
+      <c r="W167" s="28"/>
     </row>
     <row r="168" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W168" s="44"/>
+      <c r="W168" s="28"/>
     </row>
     <row r="169" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W169" s="44"/>
+      <c r="W169" s="28"/>
     </row>
     <row r="170" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W170" s="44"/>
+      <c r="W170" s="28"/>
     </row>
     <row r="171" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W171" s="44"/>
+      <c r="W171" s="28"/>
     </row>
     <row r="172" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W172" s="44"/>
+      <c r="W172" s="28"/>
     </row>
     <row r="173" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W173" s="44"/>
+      <c r="W173" s="28"/>
     </row>
     <row r="174" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W174" s="44"/>
+      <c r="W174" s="28"/>
     </row>
     <row r="175" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W175" s="44"/>
+      <c r="W175" s="28"/>
     </row>
     <row r="176" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W176" s="44"/>
+      <c r="W176" s="28"/>
     </row>
     <row r="177" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W177" s="44"/>
+      <c r="W177" s="28"/>
     </row>
     <row r="178" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W178" s="44"/>
+      <c r="W178" s="28"/>
     </row>
     <row r="179" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W179" s="44"/>
+      <c r="W179" s="28"/>
     </row>
     <row r="180" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W180" s="44"/>
+      <c r="W180" s="28"/>
     </row>
     <row r="181" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W181" s="44"/>
+      <c r="W181" s="28"/>
     </row>
     <row r="182" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W182" s="44"/>
+      <c r="W182" s="28"/>
     </row>
     <row r="183" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W183" s="44"/>
+      <c r="W183" s="28"/>
     </row>
     <row r="184" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W184" s="44"/>
+      <c r="W184" s="28"/>
     </row>
     <row r="185" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W185" s="44"/>
+      <c r="W185" s="28"/>
     </row>
     <row r="186" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W186" s="44"/>
+      <c r="W186" s="28"/>
     </row>
     <row r="187" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W187" s="44"/>
+      <c r="W187" s="28"/>
     </row>
     <row r="188" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W188" s="44"/>
+      <c r="W188" s="28"/>
     </row>
     <row r="189" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W189" s="44"/>
+      <c r="W189" s="28"/>
     </row>
     <row r="190" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W190" s="44"/>
+      <c r="W190" s="28"/>
     </row>
     <row r="191" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W191" s="44"/>
+      <c r="W191" s="28"/>
     </row>
     <row r="192" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W192" s="44"/>
+      <c r="W192" s="28"/>
     </row>
     <row r="193" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W193" s="44"/>
+      <c r="W193" s="28"/>
     </row>
     <row r="194" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W194" s="44"/>
+      <c r="W194" s="28"/>
     </row>
     <row r="195" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W195" s="44"/>
+      <c r="W195" s="28"/>
     </row>
     <row r="196" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W196" s="44"/>
+      <c r="W196" s="28"/>
     </row>
     <row r="197" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W197" s="44"/>
+      <c r="W197" s="28"/>
     </row>
     <row r="198" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W198" s="44"/>
+      <c r="W198" s="28"/>
     </row>
     <row r="199" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W199" s="44"/>
+      <c r="W199" s="28"/>
     </row>
     <row r="200" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W200" s="44"/>
+      <c r="W200" s="28"/>
     </row>
     <row r="201" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W201" s="44"/>
+      <c r="W201" s="28"/>
     </row>
     <row r="202" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W202" s="44"/>
+      <c r="W202" s="28"/>
     </row>
     <row r="203" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W203" s="44"/>
+      <c r="W203" s="28"/>
     </row>
     <row r="204" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W204" s="44"/>
+      <c r="W204" s="28"/>
     </row>
     <row r="205" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W205" s="44"/>
+      <c r="W205" s="28"/>
     </row>
     <row r="206" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W206" s="44"/>
+      <c r="W206" s="28"/>
     </row>
     <row r="207" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W207" s="44"/>
+      <c r="W207" s="28"/>
     </row>
     <row r="208" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W208" s="44"/>
+      <c r="W208" s="28"/>
     </row>
     <row r="209" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W209" s="44"/>
+      <c r="W209" s="28"/>
     </row>
     <row r="210" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W210" s="44"/>
+      <c r="W210" s="28"/>
     </row>
     <row r="211" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W211" s="44"/>
+      <c r="W211" s="28"/>
     </row>
     <row r="212" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W212" s="44"/>
+      <c r="W212" s="28"/>
     </row>
     <row r="213" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W213" s="44"/>
+      <c r="W213" s="28"/>
     </row>
     <row r="214" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W214" s="44"/>
+      <c r="W214" s="28"/>
     </row>
     <row r="215" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W215" s="44"/>
+      <c r="W215" s="28"/>
     </row>
     <row r="216" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W216" s="44"/>
+      <c r="W216" s="28"/>
     </row>
     <row r="217" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W217" s="44"/>
+      <c r="W217" s="28"/>
     </row>
     <row r="218" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W218" s="44"/>
+      <c r="W218" s="28"/>
     </row>
     <row r="219" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W219" s="44"/>
+      <c r="W219" s="28"/>
     </row>
     <row r="220" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W220" s="44"/>
+      <c r="W220" s="28"/>
     </row>
     <row r="221" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W221" s="44"/>
+      <c r="W221" s="28"/>
     </row>
     <row r="222" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W222" s="44"/>
+      <c r="W222" s="28"/>
     </row>
     <row r="223" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W223" s="44"/>
+      <c r="W223" s="28"/>
     </row>
     <row r="224" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W224" s="44"/>
+      <c r="W224" s="28"/>
     </row>
     <row r="225" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W225" s="44"/>
+      <c r="W225" s="28"/>
     </row>
     <row r="226" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W226" s="44"/>
+      <c r="W226" s="28"/>
     </row>
     <row r="227" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W227" s="44"/>
+      <c r="W227" s="28"/>
     </row>
     <row r="228" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W228" s="44"/>
+      <c r="W228" s="28"/>
     </row>
     <row r="229" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W229" s="44"/>
+      <c r="W229" s="28"/>
     </row>
     <row r="230" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W230" s="44"/>
+      <c r="W230" s="28"/>
     </row>
     <row r="231" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W231" s="44"/>
+      <c r="W231" s="28"/>
     </row>
     <row r="232" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W232" s="44"/>
+      <c r="W232" s="28"/>
     </row>
     <row r="233" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W233" s="44"/>
+      <c r="W233" s="28"/>
     </row>
     <row r="234" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W234" s="44"/>
+      <c r="W234" s="28"/>
     </row>
     <row r="235" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W235" s="44"/>
+      <c r="W235" s="28"/>
     </row>
     <row r="236" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W236" s="44"/>
+      <c r="W236" s="28"/>
     </row>
     <row r="237" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W237" s="44"/>
+      <c r="W237" s="28"/>
     </row>
     <row r="238" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W238" s="44"/>
+      <c r="W238" s="28"/>
     </row>
     <row r="239" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W239" s="44"/>
+      <c r="W239" s="28"/>
     </row>
     <row r="240" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W240" s="44"/>
+      <c r="W240" s="28"/>
     </row>
     <row r="241" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W241" s="44"/>
+      <c r="W241" s="28"/>
     </row>
     <row r="242" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W242" s="44"/>
+      <c r="W242" s="28"/>
     </row>
     <row r="243" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W243" s="44"/>
+      <c r="W243" s="28"/>
     </row>
     <row r="244" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W244" s="44"/>
+      <c r="W244" s="28"/>
     </row>
     <row r="245" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W245" s="44"/>
+      <c r="W245" s="28"/>
     </row>
     <row r="246" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W246" s="44"/>
+      <c r="W246" s="28"/>
     </row>
     <row r="247" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W247" s="44"/>
+      <c r="W247" s="28"/>
     </row>
     <row r="248" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W248" s="44"/>
+      <c r="W248" s="28"/>
     </row>
     <row r="249" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W249" s="44"/>
+      <c r="W249" s="28"/>
     </row>
     <row r="250" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W250" s="44"/>
+      <c r="W250" s="28"/>
     </row>
     <row r="251" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W251" s="44"/>
+      <c r="W251" s="28"/>
     </row>
     <row r="252" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W252" s="44"/>
+      <c r="W252" s="28"/>
     </row>
     <row r="253" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W253" s="44"/>
+      <c r="W253" s="28"/>
     </row>
     <row r="254" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W254" s="44"/>
+      <c r="W254" s="28"/>
     </row>
     <row r="255" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W255" s="44"/>
+      <c r="W255" s="28"/>
     </row>
     <row r="256" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W256" s="44"/>
+      <c r="W256" s="28"/>
     </row>
     <row r="257" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W257" s="44"/>
+      <c r="W257" s="28"/>
     </row>
     <row r="258" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W258" s="44"/>
+      <c r="W258" s="28"/>
     </row>
     <row r="259" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W259" s="44"/>
+      <c r="W259" s="28"/>
     </row>
     <row r="260" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W260" s="44"/>
+      <c r="W260" s="28"/>
     </row>
     <row r="261" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W261" s="44"/>
+      <c r="W261" s="28"/>
     </row>
     <row r="262" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W262" s="44"/>
+      <c r="W262" s="28"/>
     </row>
     <row r="263" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W263" s="44"/>
+      <c r="W263" s="28"/>
     </row>
     <row r="264" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W264" s="44"/>
+      <c r="W264" s="28"/>
     </row>
     <row r="265" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W265" s="44"/>
+      <c r="W265" s="28"/>
     </row>
     <row r="266" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W266" s="44"/>
+      <c r="W266" s="28"/>
     </row>
     <row r="267" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W267" s="44"/>
+      <c r="W267" s="28"/>
     </row>
     <row r="268" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W268" s="44"/>
+      <c r="W268" s="28"/>
     </row>
     <row r="269" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W269" s="44"/>
+      <c r="W269" s="28"/>
     </row>
     <row r="270" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W270" s="44"/>
+      <c r="W270" s="28"/>
     </row>
     <row r="271" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W271" s="44"/>
+      <c r="W271" s="28"/>
     </row>
     <row r="272" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W272" s="44"/>
+      <c r="W272" s="28"/>
     </row>
     <row r="273" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W273" s="44"/>
+      <c r="W273" s="28"/>
     </row>
     <row r="274" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W274" s="44"/>
+      <c r="W274" s="28"/>
     </row>
     <row r="275" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W275" s="44"/>
+      <c r="W275" s="28"/>
     </row>
     <row r="276" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W276" s="44"/>
+      <c r="W276" s="28"/>
     </row>
     <row r="277" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W277" s="44"/>
+      <c r="W277" s="28"/>
     </row>
     <row r="278" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W278" s="44"/>
+      <c r="W278" s="28"/>
     </row>
     <row r="279" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W279" s="44"/>
+      <c r="W279" s="28"/>
     </row>
     <row r="280" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W280" s="44"/>
+      <c r="W280" s="28"/>
     </row>
     <row r="281" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W281" s="44"/>
+      <c r="W281" s="28"/>
     </row>
     <row r="282" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W282" s="44"/>
+      <c r="W282" s="28"/>
     </row>
     <row r="283" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W283" s="44"/>
+      <c r="W283" s="28"/>
     </row>
     <row r="284" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W284" s="44"/>
+      <c r="W284" s="28"/>
     </row>
     <row r="285" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W285" s="44"/>
+      <c r="W285" s="28"/>
     </row>
     <row r="286" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W286" s="44"/>
+      <c r="W286" s="28"/>
     </row>
     <row r="287" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W287" s="44"/>
+      <c r="W287" s="28"/>
     </row>
     <row r="288" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W288" s="44"/>
+      <c r="W288" s="28"/>
     </row>
     <row r="289" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W289" s="44"/>
+      <c r="W289" s="28"/>
     </row>
     <row r="290" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W290" s="44"/>
+      <c r="W290" s="28"/>
     </row>
     <row r="291" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W291" s="44"/>
+      <c r="W291" s="28"/>
     </row>
     <row r="292" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W292" s="44"/>
+      <c r="W292" s="28"/>
     </row>
     <row r="293" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W293" s="44"/>
+      <c r="W293" s="28"/>
     </row>
     <row r="294" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W294" s="44"/>
+      <c r="W294" s="28"/>
     </row>
     <row r="295" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W295" s="44"/>
+      <c r="W295" s="28"/>
     </row>
     <row r="296" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W296" s="44"/>
+      <c r="W296" s="28"/>
     </row>
     <row r="297" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W297" s="44"/>
+      <c r="W297" s="28"/>
     </row>
     <row r="298" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W298" s="44"/>
+      <c r="W298" s="28"/>
     </row>
     <row r="299" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W299" s="44"/>
+      <c r="W299" s="28"/>
     </row>
     <row r="300" spans="23:23" x14ac:dyDescent="0.2">
-      <c r="W300" s="44"/>
+      <c r="W300" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="G22:H50"/>
+    <mergeCell ref="D22:F24"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="D34:F41"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="K33:K36"/>
     <mergeCell ref="AR4:AT4"/>
     <mergeCell ref="M15:M20"/>
     <mergeCell ref="J12:J15"/>
@@ -5219,13 +5304,6 @@
     <mergeCell ref="E12:E16"/>
     <mergeCell ref="F12:F16"/>
     <mergeCell ref="G15:G17"/>
-    <mergeCell ref="G22:H50"/>
-    <mergeCell ref="D22:F24"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="D34:F41"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="K33:K36"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>